<commit_message>
feat(Salary): edit export excel salary
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/salary_month.xlsx
+++ b/src/storage/app/excel-exporter/templates/salary_month.xlsx
@@ -758,9 +758,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
-  <si>
-    <t xml:space="preserve">      CHẤN THANH</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
+  <si>
+    <t xml:space="preserve">CHẤN THANH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BẢNG LƯƠNG THÁNG {month}</t>
   </si>
   <si>
     <t xml:space="preserve">Ngày công chuẩn</t>
@@ -773,6 +776,9 @@
   </si>
   <si>
     <t xml:space="preserve">{end_time}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Từ {start_time} đến {end_time} {from_to}</t>
   </si>
   <si>
     <t xml:space="preserve">Mức lương trần Bảo Hiểm Xã Hội</t>
@@ -893,6 +899,82 @@
   <si>
     <t xml:space="preserve">Note
 {c_note}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{c_empty_1}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ký cam kết {c_month_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">sign_commitment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}/TNCN </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Lưu ý thời gian thử việc
+{c_probationary_note}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{c_empty_2}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">LƯƠNG TRÊN MỖI GIỜ LÀM VIỆC
+{c_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">salary_hours</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">{c_merge_ot_empty}</t>
   </si>
   <si>
     <t xml:space="preserve">[[basic_salary_allowance]]</t>
@@ -1034,6 +1116,95 @@
 {c_advance}</t>
   </si>
   <si>
+    <t xml:space="preserve">OVERTIME{c_over_time}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OT taxable
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">{c_ot_tax_2}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">OT Non-tax
+{c_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">ot_no_tax_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Total OT amount
+{c_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">total_ot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">[number]</t>
   </si>
   <si>
@@ -1137,6 +1308,36 @@
   </si>
   <si>
     <t xml:space="preserve">[note]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[empty_1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[sign_commitment]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[probationary_period]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[empty_2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[salary_hours]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ot_weekday]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ot_weekend]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ot_holiday]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[total_hour_ot]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[total_ot]</t>
   </si>
   <si>
     <t xml:space="preserve">TỔNG CỘNG
@@ -1902,7 +2103,16 @@
     <t xml:space="preserve">PHÒNG HÀNH CHÍNH</t>
   </si>
   <si>
+    <t xml:space="preserve">TPHCM, ngày {date_sign} tháng {month_sign} năm {year_sign}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIÁM ĐỐC</t>
+  </si>
+  <si>
     <t xml:space="preserve">NGUYỄN THỊ HỒNG AN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGUYỄN HUỲNH THU TRÚC</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +2128,7 @@
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1960,6 +2170,14 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -2013,12 +2231,31 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -2134,7 +2371,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2167,11 +2404,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2187,23 +2428,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2219,7 +2460,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2231,15 +2472,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2247,7 +2488,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2267,15 +2512,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2299,35 +2544,51 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2414,7 +2675,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2428,7 +2689,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="9" style="1" width="11.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="974" min="36" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="46" min="36" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="15.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="974" min="48" style="1" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="975" style="1" width="10.5"/>
   </cols>
   <sheetData>
@@ -2446,10 +2709,10 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2470,588 +2733,632 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="8" t="s">
+        <v>1</v>
+      </c>
       <c r="K3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="5"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="13" t="n">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="14" t="n">
         <v>149000</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="18"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="19"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
       <c r="I10" s="5"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
-      <c r="B11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="F11" s="6" t="n">
-        <v>5</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="I11" s="6" t="n">
-        <v>7</v>
-      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="6"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" s="28" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="20" t="s">
+    <row r="12" s="29" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="C12" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="D12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="E12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="F12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="G12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="H12" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="I12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="J12" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="22"/>
-      <c r="N12" s="24" t="s">
+      <c r="K12" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="O12" s="22" t="s">
+      <c r="L12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="P12" s="22" t="s">
+      <c r="M12" s="23"/>
+      <c r="N12" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="Q12" s="22" t="s">
+      <c r="O12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22" t="s">
+      <c r="P12" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22"/>
-      <c r="Y12" s="22"/>
-      <c r="Z12" s="22" t="s">
+      <c r="Q12" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="AA12" s="22"/>
-      <c r="AB12" s="22"/>
-      <c r="AC12" s="22" t="s">
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="AD12" s="22" t="s">
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="AE12" s="25" t="s">
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="AF12" s="22" t="s">
+      <c r="AD12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="AG12" s="24"/>
-      <c r="AH12" s="26" t="s">
+      <c r="AE12" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AI12" s="27" t="s">
+      <c r="AF12" s="23" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" s="28" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="20" t="s">
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="AI12" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22" t="s">
+      <c r="AJ12" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="22" t="s">
+      <c r="AK12" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22" t="s">
+      <c r="AL12" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="R13" s="22" t="s">
+      <c r="AM12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="S13" s="22" t="s">
+      <c r="AN12" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="T13" s="22" t="s">
+      <c r="AO12" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="U13" s="22" t="s">
+    </row>
+    <row r="13" s="29" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="V13" s="22" t="s">
+      <c r="J13" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="W13" s="22" t="s">
+      <c r="K13" s="23"/>
+      <c r="L13" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="X13" s="22" t="s">
+      <c r="M13" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="Y13" s="22" t="s">
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="Z13" s="22" t="s">
+      <c r="R13" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="AA13" s="22" t="s">
+      <c r="S13" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="AB13" s="22" t="s">
+      <c r="T13" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="AC13" s="22"/>
-      <c r="AD13" s="22"/>
-      <c r="AE13" s="22"/>
-      <c r="AF13" s="22" t="s">
+      <c r="U13" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AG13" s="24" t="s">
+      <c r="V13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="AH13" s="26"/>
-      <c r="AI13" s="27"/>
-    </row>
-    <row r="14" s="33" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="30"/>
-      <c r="Z14" s="30"/>
-      <c r="AA14" s="30"/>
-      <c r="AB14" s="30"/>
-      <c r="AC14" s="30"/>
-      <c r="AD14" s="30"/>
-      <c r="AE14" s="30"/>
-      <c r="AF14" s="30"/>
-      <c r="AG14" s="30"/>
-      <c r="AH14" s="30"/>
-      <c r="AI14" s="30"/>
-      <c r="AMJ14" s="34"/>
-    </row>
-    <row r="15" s="42" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="s">
+      <c r="W13" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="X13" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="Y13" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="Z13" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="AA13" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="AB13" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="23"/>
+      <c r="AF13" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="AG13" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="39" t="s">
+      <c r="AH13" s="27"/>
+      <c r="AI13" s="28"/>
+      <c r="AO13" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="AS13" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="38" t="s">
+      <c r="AT13" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="AU13" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="M15" s="38" t="s">
+    </row>
+    <row r="14" s="35" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
+      <c r="AD14" s="32"/>
+      <c r="AE14" s="32"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="32"/>
+      <c r="AMJ14" s="36"/>
+    </row>
+    <row r="15" s="44" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="N15" s="39" t="s">
+      <c r="B15" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="O15" s="38" t="s">
+      <c r="C15" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="D15" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="Q15" s="38" t="s">
+      <c r="E15" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="R15" s="38" t="s">
+      <c r="F15" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="S15" s="38" t="s">
+      <c r="G15" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="T15" s="38" t="s">
+      <c r="H15" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="U15" s="38" t="s">
+      <c r="I15" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="V15" s="38" t="s">
+      <c r="J15" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="W15" s="38" t="s">
+      <c r="K15" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="X15" s="38" t="s">
+      <c r="L15" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="Y15" s="38" t="s">
+      <c r="M15" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="Z15" s="38" t="s">
+      <c r="N15" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="AA15" s="38" t="s">
+      <c r="O15" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="AB15" s="38" t="s">
+      <c r="P15" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="AC15" s="38" t="s">
+      <c r="Q15" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="AD15" s="38" t="s">
+      <c r="R15" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="AE15" s="38" t="s">
+      <c r="S15" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="AF15" s="38" t="s">
+      <c r="T15" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="AG15" s="38" t="s">
+      <c r="U15" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="AH15" s="38" t="s">
+      <c r="V15" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="AI15" s="40" t="s">
+      <c r="W15" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="AJ15" s="41"/>
-      <c r="AK15" s="41"/>
-      <c r="AL15" s="41"/>
-      <c r="AM15" s="41"/>
-      <c r="AN15" s="41"/>
-      <c r="AO15" s="41"/>
-      <c r="AP15" s="41"/>
-      <c r="AQ15" s="41"/>
-      <c r="AR15" s="41"/>
-      <c r="AS15" s="41"/>
-      <c r="AT15" s="41"/>
-      <c r="AU15" s="41"/>
-      <c r="AV15" s="41"/>
-      <c r="AW15" s="41"/>
-      <c r="AX15" s="41"/>
-      <c r="AY15" s="41"/>
-      <c r="AZ15" s="41"/>
-      <c r="BA15" s="41"/>
-      <c r="BB15" s="41"/>
-      <c r="BC15" s="41"/>
-      <c r="BD15" s="41"/>
-      <c r="BE15" s="41"/>
-      <c r="BF15" s="41"/>
-      <c r="BG15" s="41"/>
-      <c r="BH15" s="41"/>
-      <c r="BI15" s="41"/>
-      <c r="BJ15" s="41"/>
-      <c r="BK15" s="41"/>
-      <c r="BL15" s="41"/>
-      <c r="BM15" s="41"/>
-      <c r="BN15" s="41"/>
-      <c r="BO15" s="41"/>
-      <c r="BP15" s="41"/>
-      <c r="BQ15" s="41"/>
-    </row>
-    <row r="16" s="47" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="43" t="s">
+      <c r="X15" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="46" t="s">
+      <c r="Y15" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I16" s="46" t="s">
+      <c r="Z15" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="46" t="s">
+      <c r="AA15" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="K16" s="46" t="s">
+      <c r="AB15" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="AC15" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="M16" s="46" t="s">
+      <c r="AD15" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="N16" s="46" t="s">
+      <c r="AE15" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="O16" s="46" t="s">
+      <c r="AF15" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="P16" s="46" t="s">
+      <c r="AG15" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="Q16" s="46" t="s">
+      <c r="AH15" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="R16" s="46" t="s">
+      <c r="AI15" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="S16" s="46" t="s">
+      <c r="AJ15" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="T16" s="46" t="s">
+      <c r="AK15" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="U16" s="46" t="s">
+      <c r="AL15" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="V16" s="46" t="s">
+      <c r="AM15" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="W16" s="46" t="s">
+      <c r="AN15" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="X16" s="46" t="s">
+      <c r="AO15" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="Y16" s="46" t="s">
+      <c r="AP15" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="Z16" s="46" t="s">
+      <c r="AQ15" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="AA16" s="46" t="s">
+      <c r="AR15" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="AB16" s="46" t="s">
+      <c r="AS15" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT15" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="AU15" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="AC16" s="46" t="s">
+      <c r="AV15" s="43"/>
+      <c r="AW15" s="43"/>
+      <c r="AX15" s="43"/>
+      <c r="AY15" s="43"/>
+      <c r="AZ15" s="43"/>
+      <c r="BA15" s="43"/>
+      <c r="BB15" s="43"/>
+      <c r="BC15" s="43"/>
+      <c r="BD15" s="43"/>
+      <c r="BE15" s="43"/>
+      <c r="BF15" s="43"/>
+      <c r="BG15" s="43"/>
+      <c r="BH15" s="43"/>
+      <c r="BI15" s="43"/>
+      <c r="BJ15" s="43"/>
+      <c r="BK15" s="43"/>
+      <c r="BL15" s="43"/>
+      <c r="BM15" s="43"/>
+      <c r="BN15" s="43"/>
+      <c r="BO15" s="43"/>
+      <c r="BP15" s="43"/>
+      <c r="BQ15" s="43"/>
+    </row>
+    <row r="16" s="49" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="AD16" s="46" t="s">
+      <c r="B16" s="46"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="AE16" s="46" t="s">
+      <c r="I16" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="AF16" s="46" t="s">
+      <c r="J16" s="48" t="s">
         <v>118</v>
       </c>
-      <c r="AG16" s="46" t="s">
+      <c r="K16" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="AH16" s="46" t="s">
+      <c r="L16" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="AI16" s="46" t="s">
+      <c r="M16" s="48" t="s">
         <v>121</v>
+      </c>
+      <c r="N16" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="O16" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="P16" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q16" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="R16" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="S16" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="T16" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="U16" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="V16" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="W16" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="X16" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y16" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z16" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA16" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB16" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC16" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD16" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE16" s="48" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF16" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG16" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH16" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI16" s="48" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3066,12 +3373,14 @@
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
+      <c r="AI17" s="50"/>
+      <c r="AJ17" s="50"/>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="2" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -3081,6 +3390,10 @@
       <c r="I18" s="5"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
+      <c r="AI18" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ18" s="50"/>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
@@ -3094,6 +3407,10 @@
       <c r="I19" s="5"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
+      <c r="AI19" s="50"/>
+      <c r="AJ19" s="52" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
@@ -3116,7 +3433,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="48"/>
+      <c r="H21" s="53"/>
       <c r="I21" s="5"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -3129,7 +3446,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="48"/>
+      <c r="H22" s="53"/>
       <c r="I22" s="5"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -3142,7 +3459,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="48"/>
+      <c r="H23" s="53"/>
       <c r="I23" s="5"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -3150,8 +3467,8 @@
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="4" t="s">
-        <v>123</v>
+      <c r="C24" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -3161,6 +3478,9 @@
       <c r="I24" s="5"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
+      <c r="AI24" s="54" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>

</xml_diff>

<commit_message>
fix(App): update feedback 11/11/2021
</commit_message>
<xml_diff>
--- a/src/storage/app/excel-exporter/templates/salary_month.xlsx
+++ b/src/storage/app/excel-exporter/templates/salary_month.xlsx
@@ -904,35 +904,7 @@
     <t xml:space="preserve">{c_empty_1}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Ký cam kết {c_month_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">sign_commitment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}/TNCN </t>
-    </r>
+    <t xml:space="preserve">Ký cam kết {c_month_sign_commitment}/TNCN </t>
   </si>
   <si>
     <t xml:space="preserve">Lưu ý thời gian thử việc
@@ -942,36 +914,8 @@
     <t xml:space="preserve">{c_empty_2}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">LƯƠNG TRÊN MỖI GIỜ LÀM VIỆC
-{c_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">salary_hours</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}</t>
-    </r>
+    <t xml:space="preserve">LƯƠNG TRÊN MỖI GIỜ LÀM VIỆC
+{c_salary_hours}</t>
   </si>
   <si>
     <t xml:space="preserve">{c_merge_ot_empty}</t>
@@ -1136,6 +1080,7 @@
         <color rgb="FF000000"/>
         <rFont val="arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">{c_ot_tax_2}</t>
     </r>
@@ -1158,6 +1103,7 @@
         <color rgb="FF000000"/>
         <rFont val="arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ot_no_tax_2</t>
     </r>
@@ -1173,36 +1119,8 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Total OT amount
-{c_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">total_ot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}</t>
-    </r>
+    <t xml:space="preserve">Total OT amount
+{c_total_ot}</t>
   </si>
   <si>
     <t xml:space="preserve">[number]</t>
@@ -2128,7 +2046,7 @@
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2231,18 +2149,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
       <charset val="1"/>
@@ -2251,8 +2157,8 @@
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -2371,37 +2277,41 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2417,23 +2327,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2449,7 +2347,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -2520,7 +2418,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2552,15 +2450,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2568,28 +2470,24 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2675,7 +2573,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="14" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2709,7 +2607,7 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2725,48 +2623,48 @@
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
@@ -2779,11 +2677,11 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="14" t="s">
         <v>10</v>
       </c>
@@ -2796,28 +2694,28 @@
       <c r="K6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="14" t="s">
         <v>14</v>
       </c>
@@ -2829,11 +2727,11 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="10"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="14" t="n">
         <v>149000</v>
       </c>
@@ -2841,16 +2739,16 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="19"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="14" t="s">
         <v>17</v>
       </c>
@@ -2864,506 +2762,506 @@
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="6"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" s="29" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
+    <row r="12" s="27" customFormat="true" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="25" t="s">
+      <c r="M12" s="21"/>
+      <c r="N12" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="O12" s="23" t="s">
+      <c r="O12" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="23" t="s">
+      <c r="P12" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="Q12" s="23" t="s">
+      <c r="Q12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23"/>
-      <c r="T12" s="23"/>
-      <c r="U12" s="23" t="s">
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23" t="s">
+      <c r="V12" s="21"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="21"/>
+      <c r="Y12" s="21"/>
+      <c r="Z12" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23" t="s">
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="21"/>
+      <c r="AC12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="AD12" s="23" t="s">
+      <c r="AD12" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AE12" s="26" t="s">
+      <c r="AE12" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="AF12" s="23" t="s">
+      <c r="AF12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AG12" s="25"/>
-      <c r="AH12" s="27" t="s">
+      <c r="AG12" s="23"/>
+      <c r="AH12" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="AI12" s="28" t="s">
+      <c r="AI12" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AJ12" s="29" t="s">
+      <c r="AJ12" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="AK12" s="30" t="s">
+      <c r="AK12" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="AL12" s="29" t="s">
+      <c r="AL12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AM12" s="29" t="s">
+      <c r="AM12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="AN12" s="29" t="s">
+      <c r="AN12" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="AO12" s="29" t="s">
+      <c r="AO12" s="27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" s="29" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="21" t="s">
+    <row r="13" s="27" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23" t="s">
+      <c r="K13" s="21"/>
+      <c r="L13" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23" t="s">
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="R13" s="23" t="s">
+      <c r="R13" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="S13" s="23" t="s">
+      <c r="S13" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="T13" s="23" t="s">
+      <c r="T13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="U13" s="23" t="s">
+      <c r="U13" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="V13" s="23" t="s">
+      <c r="V13" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="W13" s="23" t="s">
+      <c r="W13" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="X13" s="23" t="s">
+      <c r="X13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="Y13" s="23" t="s">
+      <c r="Y13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="Z13" s="23" t="s">
+      <c r="Z13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="AA13" s="23" t="s">
+      <c r="AA13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="AB13" s="23" t="s">
+      <c r="AB13" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-      <c r="AE13" s="23"/>
-      <c r="AF13" s="23" t="s">
+      <c r="AC13" s="21"/>
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="AG13" s="25" t="s">
+      <c r="AG13" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="AH13" s="27"/>
-      <c r="AI13" s="28"/>
-      <c r="AO13" s="29" t="s">
+      <c r="AH13" s="25"/>
+      <c r="AI13" s="26"/>
+      <c r="AO13" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="AS13" s="29" t="s">
+      <c r="AS13" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="AT13" s="29" t="s">
+      <c r="AT13" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="AU13" s="29" t="s">
+      <c r="AU13" s="27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" s="35" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="34"/>
-      <c r="T14" s="32"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="33"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="32"/>
-      <c r="AB14" s="32"/>
-      <c r="AC14" s="32"/>
-      <c r="AD14" s="32"/>
-      <c r="AE14" s="32"/>
-      <c r="AF14" s="32"/>
-      <c r="AG14" s="32"/>
-      <c r="AH14" s="32"/>
-      <c r="AI14" s="32"/>
-      <c r="AMJ14" s="36"/>
-    </row>
-    <row r="15" s="44" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
+    <row r="14" s="33" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="30"/>
+      <c r="AB14" s="30"/>
+      <c r="AC14" s="30"/>
+      <c r="AD14" s="30"/>
+      <c r="AE14" s="30"/>
+      <c r="AF14" s="30"/>
+      <c r="AG14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AI14" s="30"/>
+      <c r="AMJ14" s="34"/>
+    </row>
+    <row r="15" s="42" customFormat="true" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="38" t="s">
+      <c r="F15" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="I15" s="41" t="s">
+      <c r="I15" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="40" t="s">
+      <c r="J15" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="40" t="s">
+      <c r="K15" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="L15" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="41" t="s">
+      <c r="N15" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="O15" s="40" t="s">
+      <c r="O15" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="P15" s="40" t="s">
+      <c r="P15" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="Q15" s="40" t="s">
+      <c r="Q15" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="R15" s="40" t="s">
+      <c r="R15" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="S15" s="40" t="s">
+      <c r="S15" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="T15" s="40" t="s">
+      <c r="T15" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="U15" s="40" t="s">
+      <c r="U15" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="V15" s="40" t="s">
+      <c r="V15" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="W15" s="40" t="s">
+      <c r="W15" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="X15" s="40" t="s">
+      <c r="X15" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="Y15" s="40" t="s">
+      <c r="Y15" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="Z15" s="40" t="s">
+      <c r="Z15" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="AA15" s="40" t="s">
+      <c r="AA15" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="AB15" s="40" t="s">
+      <c r="AB15" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="AC15" s="40" t="s">
+      <c r="AC15" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="AD15" s="40" t="s">
+      <c r="AD15" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="AE15" s="40" t="s">
+      <c r="AE15" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="AF15" s="40" t="s">
+      <c r="AF15" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="AG15" s="40" t="s">
+      <c r="AG15" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="AH15" s="40" t="s">
+      <c r="AH15" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="AI15" s="42" t="s">
+      <c r="AI15" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="AJ15" s="43" t="s">
+      <c r="AJ15" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="AK15" s="43" t="s">
+      <c r="AK15" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="AL15" s="43" t="s">
+      <c r="AL15" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="AM15" s="43" t="s">
+      <c r="AM15" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="AN15" s="43" t="s">
+      <c r="AN15" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="AO15" s="43" t="s">
+      <c r="AO15" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="AP15" s="43" t="s">
+      <c r="AP15" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="AQ15" s="43" t="s">
+      <c r="AQ15" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="AR15" s="43" t="s">
+      <c r="AR15" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="AS15" s="40" t="s">
+      <c r="AS15" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AT15" s="40" t="s">
+      <c r="AT15" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="AU15" s="43" t="s">
+      <c r="AU15" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="AV15" s="43"/>
-      <c r="AW15" s="43"/>
-      <c r="AX15" s="43"/>
-      <c r="AY15" s="43"/>
-      <c r="AZ15" s="43"/>
-      <c r="BA15" s="43"/>
-      <c r="BB15" s="43"/>
-      <c r="BC15" s="43"/>
-      <c r="BD15" s="43"/>
-      <c r="BE15" s="43"/>
-      <c r="BF15" s="43"/>
-      <c r="BG15" s="43"/>
-      <c r="BH15" s="43"/>
-      <c r="BI15" s="43"/>
-      <c r="BJ15" s="43"/>
-      <c r="BK15" s="43"/>
-      <c r="BL15" s="43"/>
-      <c r="BM15" s="43"/>
-      <c r="BN15" s="43"/>
-      <c r="BO15" s="43"/>
-      <c r="BP15" s="43"/>
-      <c r="BQ15" s="43"/>
-    </row>
-    <row r="16" s="49" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
+      <c r="AV15" s="41"/>
+      <c r="AW15" s="41"/>
+      <c r="AX15" s="41"/>
+      <c r="AY15" s="41"/>
+      <c r="AZ15" s="41"/>
+      <c r="BA15" s="41"/>
+      <c r="BB15" s="41"/>
+      <c r="BC15" s="41"/>
+      <c r="BD15" s="41"/>
+      <c r="BE15" s="41"/>
+      <c r="BF15" s="41"/>
+      <c r="BG15" s="41"/>
+      <c r="BH15" s="41"/>
+      <c r="BI15" s="41"/>
+      <c r="BJ15" s="41"/>
+      <c r="BK15" s="41"/>
+      <c r="BL15" s="41"/>
+      <c r="BM15" s="41"/>
+      <c r="BN15" s="41"/>
+      <c r="BO15" s="41"/>
+      <c r="BP15" s="41"/>
+      <c r="BQ15" s="41"/>
+    </row>
+    <row r="16" s="48" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="J16" s="48" t="s">
+      <c r="J16" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="L16" s="48" t="s">
+      <c r="L16" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="M16" s="48" t="s">
+      <c r="M16" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="N16" s="48" t="s">
+      <c r="N16" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="O16" s="48" t="s">
+      <c r="O16" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="P16" s="48" t="s">
+      <c r="P16" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="Q16" s="48" t="s">
+      <c r="Q16" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="R16" s="48" t="s">
+      <c r="R16" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="S16" s="48" t="s">
+      <c r="S16" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="T16" s="48" t="s">
+      <c r="T16" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="U16" s="48" t="s">
+      <c r="U16" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="V16" s="48" t="s">
+      <c r="V16" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="W16" s="48" t="s">
+      <c r="W16" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="X16" s="48" t="s">
+      <c r="X16" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="Y16" s="48" t="s">
+      <c r="Y16" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="Z16" s="48" t="s">
+      <c r="Z16" s="47" t="s">
         <v>134</v>
       </c>
-      <c r="AA16" s="48" t="s">
+      <c r="AA16" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="AB16" s="48" t="s">
+      <c r="AB16" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="AC16" s="48" t="s">
+      <c r="AC16" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="AD16" s="48" t="s">
+      <c r="AD16" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="AE16" s="48" t="s">
+      <c r="AE16" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="AF16" s="48" t="s">
+      <c r="AF16" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="AG16" s="48" t="s">
+      <c r="AG16" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="AH16" s="48" t="s">
+      <c r="AH16" s="46" t="s">
         <v>142</v>
       </c>
-      <c r="AI16" s="48" t="s">
+      <c r="AI16" s="47" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -3373,12 +3271,12 @@
       <c r="I17" s="5"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="AI17" s="50"/>
-      <c r="AJ17" s="50"/>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="49"/>
     </row>
     <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="2" t="s">
         <v>144</v>
       </c>
@@ -3390,14 +3288,14 @@
       <c r="I18" s="5"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="AI18" s="51" t="s">
+      <c r="AI18" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="AJ18" s="50"/>
+      <c r="AJ18" s="49"/>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -3407,14 +3305,14 @@
       <c r="I19" s="5"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="AI19" s="50"/>
-      <c r="AJ19" s="52" t="s">
+      <c r="AI19" s="49"/>
+      <c r="AJ19" s="51" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -3427,46 +3325,46 @@
     </row>
     <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="53"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="5"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="53"/>
+      <c r="H22" s="4"/>
       <c r="I22" s="5"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="53"/>
+      <c r="H23" s="4"/>
       <c r="I23" s="5"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="2" t="s">
         <v>147</v>
       </c>
@@ -3478,13 +3376,13 @@
       <c r="I24" s="5"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="AI24" s="54" t="s">
+      <c r="AI24" s="52" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="7"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -3497,7 +3395,7 @@
     </row>
     <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -3510,7 +3408,7 @@
     </row>
     <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -3523,7 +3421,7 @@
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -3536,7 +3434,7 @@
     </row>
     <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -3549,7 +3447,7 @@
     </row>
     <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -3562,7 +3460,7 @@
     </row>
     <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="7"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -3575,7 +3473,7 @@
     </row>
     <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -3588,7 +3486,7 @@
     </row>
     <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
-      <c r="B33" s="6"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -3601,7 +3499,7 @@
     </row>
     <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
-      <c r="B34" s="6"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -3614,7 +3512,7 @@
     </row>
     <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
-      <c r="B35" s="6"/>
+      <c r="B35" s="7"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -3627,7 +3525,7 @@
     </row>
     <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
-      <c r="B36" s="6"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -3640,7 +3538,7 @@
     </row>
     <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
-      <c r="B37" s="6"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -3653,7 +3551,7 @@
     </row>
     <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
-      <c r="B38" s="6"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -3666,7 +3564,7 @@
     </row>
     <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
-      <c r="B39" s="6"/>
+      <c r="B39" s="7"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -3679,7 +3577,7 @@
     </row>
     <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
-      <c r="B40" s="6"/>
+      <c r="B40" s="7"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -3692,7 +3590,7 @@
     </row>
     <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
-      <c r="B41" s="6"/>
+      <c r="B41" s="7"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -3705,7 +3603,7 @@
     </row>
     <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
-      <c r="B42" s="6"/>
+      <c r="B42" s="7"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -3718,7 +3616,7 @@
     </row>
     <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
-      <c r="B43" s="6"/>
+      <c r="B43" s="7"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -3731,7 +3629,7 @@
     </row>
     <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
-      <c r="B44" s="6"/>
+      <c r="B44" s="7"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -3744,7 +3642,7 @@
     </row>
     <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
-      <c r="B45" s="6"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -3757,7 +3655,7 @@
     </row>
     <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
-      <c r="B46" s="6"/>
+      <c r="B46" s="7"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -3770,7 +3668,7 @@
     </row>
     <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
-      <c r="B47" s="6"/>
+      <c r="B47" s="7"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -3783,7 +3681,7 @@
     </row>
     <row r="48" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
-      <c r="B48" s="6"/>
+      <c r="B48" s="7"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -3796,7 +3694,7 @@
     </row>
     <row r="49" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
-      <c r="B49" s="6"/>
+      <c r="B49" s="7"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -3809,7 +3707,7 @@
     </row>
     <row r="50" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
-      <c r="B50" s="6"/>
+      <c r="B50" s="7"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -3822,7 +3720,7 @@
     </row>
     <row r="51" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
-      <c r="B51" s="6"/>
+      <c r="B51" s="7"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -3835,7 +3733,7 @@
     </row>
     <row r="52" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
-      <c r="B52" s="6"/>
+      <c r="B52" s="7"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -3848,7 +3746,7 @@
     </row>
     <row r="53" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
-      <c r="B53" s="6"/>
+      <c r="B53" s="7"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -3861,7 +3759,7 @@
     </row>
     <row r="54" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
-      <c r="B54" s="6"/>
+      <c r="B54" s="7"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -3874,7 +3772,7 @@
     </row>
     <row r="55" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="4"/>
-      <c r="B55" s="6"/>
+      <c r="B55" s="7"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -3887,7 +3785,7 @@
     </row>
     <row r="56" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="4"/>
-      <c r="B56" s="6"/>
+      <c r="B56" s="7"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -3900,7 +3798,7 @@
     </row>
     <row r="57" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="4"/>
-      <c r="B57" s="6"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -3913,7 +3811,7 @@
     </row>
     <row r="58" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="4"/>
-      <c r="B58" s="6"/>
+      <c r="B58" s="7"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -3926,7 +3824,7 @@
     </row>
     <row r="59" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="4"/>
-      <c r="B59" s="6"/>
+      <c r="B59" s="7"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -3939,7 +3837,7 @@
     </row>
     <row r="60" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
-      <c r="B60" s="6"/>
+      <c r="B60" s="7"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -3952,7 +3850,7 @@
     </row>
     <row r="61" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
-      <c r="B61" s="6"/>
+      <c r="B61" s="7"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -3965,7 +3863,7 @@
     </row>
     <row r="62" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="4"/>
-      <c r="B62" s="6"/>
+      <c r="B62" s="7"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -3978,7 +3876,7 @@
     </row>
     <row r="63" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="4"/>
-      <c r="B63" s="6"/>
+      <c r="B63" s="7"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -3991,7 +3889,7 @@
     </row>
     <row r="64" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="4"/>
-      <c r="B64" s="6"/>
+      <c r="B64" s="7"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -4004,7 +3902,7 @@
     </row>
     <row r="65" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="4"/>
-      <c r="B65" s="6"/>
+      <c r="B65" s="7"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -4017,7 +3915,7 @@
     </row>
     <row r="66" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="4"/>
-      <c r="B66" s="6"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -4030,7 +3928,7 @@
     </row>
     <row r="67" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="4"/>
-      <c r="B67" s="6"/>
+      <c r="B67" s="7"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -4043,7 +3941,7 @@
     </row>
     <row r="68" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
-      <c r="B68" s="6"/>
+      <c r="B68" s="7"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -4056,7 +3954,7 @@
     </row>
     <row r="69" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
-      <c r="B69" s="6"/>
+      <c r="B69" s="7"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -4069,7 +3967,7 @@
     </row>
     <row r="70" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
-      <c r="B70" s="6"/>
+      <c r="B70" s="7"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -4082,7 +3980,7 @@
     </row>
     <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="4"/>
-      <c r="B71" s="6"/>
+      <c r="B71" s="7"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -4095,7 +3993,7 @@
     </row>
     <row r="72" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="4"/>
-      <c r="B72" s="6"/>
+      <c r="B72" s="7"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -4108,7 +4006,7 @@
     </row>
     <row r="73" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="4"/>
-      <c r="B73" s="6"/>
+      <c r="B73" s="7"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -4121,7 +4019,7 @@
     </row>
     <row r="74" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="4"/>
-      <c r="B74" s="6"/>
+      <c r="B74" s="7"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -4134,7 +4032,7 @@
     </row>
     <row r="75" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="4"/>
-      <c r="B75" s="6"/>
+      <c r="B75" s="7"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -4147,7 +4045,7 @@
     </row>
     <row r="76" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
-      <c r="B76" s="6"/>
+      <c r="B76" s="7"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -4160,7 +4058,7 @@
     </row>
     <row r="77" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
-      <c r="B77" s="6"/>
+      <c r="B77" s="7"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -4173,7 +4071,7 @@
     </row>
     <row r="78" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="4"/>
-      <c r="B78" s="6"/>
+      <c r="B78" s="7"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -4186,7 +4084,7 @@
     </row>
     <row r="79" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="4"/>
-      <c r="B79" s="6"/>
+      <c r="B79" s="7"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -4199,7 +4097,7 @@
     </row>
     <row r="80" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="4"/>
-      <c r="B80" s="6"/>
+      <c r="B80" s="7"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -4212,7 +4110,7 @@
     </row>
     <row r="81" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="4"/>
-      <c r="B81" s="6"/>
+      <c r="B81" s="7"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -4225,7 +4123,7 @@
     </row>
     <row r="82" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="4"/>
-      <c r="B82" s="6"/>
+      <c r="B82" s="7"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -4238,7 +4136,7 @@
     </row>
     <row r="83" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="4"/>
-      <c r="B83" s="6"/>
+      <c r="B83" s="7"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -4251,7 +4149,7 @@
     </row>
     <row r="84" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="4"/>
-      <c r="B84" s="6"/>
+      <c r="B84" s="7"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -4264,7 +4162,7 @@
     </row>
     <row r="85" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="4"/>
-      <c r="B85" s="6"/>
+      <c r="B85" s="7"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -4277,7 +4175,7 @@
     </row>
     <row r="86" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="4"/>
-      <c r="B86" s="6"/>
+      <c r="B86" s="7"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -4290,7 +4188,7 @@
     </row>
     <row r="87" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="4"/>
-      <c r="B87" s="6"/>
+      <c r="B87" s="7"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -4303,7 +4201,7 @@
     </row>
     <row r="88" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="4"/>
-      <c r="B88" s="6"/>
+      <c r="B88" s="7"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -4316,7 +4214,7 @@
     </row>
     <row r="89" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="4"/>
-      <c r="B89" s="6"/>
+      <c r="B89" s="7"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -4329,7 +4227,7 @@
     </row>
     <row r="90" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="4"/>
-      <c r="B90" s="6"/>
+      <c r="B90" s="7"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -4342,7 +4240,7 @@
     </row>
     <row r="91" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="4"/>
-      <c r="B91" s="6"/>
+      <c r="B91" s="7"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -4355,7 +4253,7 @@
     </row>
     <row r="92" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="4"/>
-      <c r="B92" s="6"/>
+      <c r="B92" s="7"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -4368,7 +4266,7 @@
     </row>
     <row r="93" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="4"/>
-      <c r="B93" s="6"/>
+      <c r="B93" s="7"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -4381,7 +4279,7 @@
     </row>
     <row r="94" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="4"/>
-      <c r="B94" s="6"/>
+      <c r="B94" s="7"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -4394,7 +4292,7 @@
     </row>
     <row r="95" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="4"/>
-      <c r="B95" s="6"/>
+      <c r="B95" s="7"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -4407,7 +4305,7 @@
     </row>
     <row r="96" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="4"/>
-      <c r="B96" s="6"/>
+      <c r="B96" s="7"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -4420,7 +4318,7 @@
     </row>
     <row r="97" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="4"/>
-      <c r="B97" s="6"/>
+      <c r="B97" s="7"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -4433,7 +4331,7 @@
     </row>
     <row r="98" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="4"/>
-      <c r="B98" s="6"/>
+      <c r="B98" s="7"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -4446,7 +4344,7 @@
     </row>
     <row r="99" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="4"/>
-      <c r="B99" s="6"/>
+      <c r="B99" s="7"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -4459,7 +4357,7 @@
     </row>
     <row r="100" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="4"/>
-      <c r="B100" s="6"/>
+      <c r="B100" s="7"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -4472,7 +4370,7 @@
     </row>
     <row r="101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="4"/>
-      <c r="B101" s="6"/>
+      <c r="B101" s="7"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -4485,7 +4383,7 @@
     </row>
     <row r="102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="4"/>
-      <c r="B102" s="6"/>
+      <c r="B102" s="7"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -4498,7 +4396,7 @@
     </row>
     <row r="103" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="4"/>
-      <c r="B103" s="6"/>
+      <c r="B103" s="7"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -4511,7 +4409,7 @@
     </row>
     <row r="104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="4"/>
-      <c r="B104" s="6"/>
+      <c r="B104" s="7"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -4524,7 +4422,7 @@
     </row>
     <row r="105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="4"/>
-      <c r="B105" s="6"/>
+      <c r="B105" s="7"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -4537,7 +4435,7 @@
     </row>
     <row r="106" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="4"/>
-      <c r="B106" s="6"/>
+      <c r="B106" s="7"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -4550,7 +4448,7 @@
     </row>
     <row r="107" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="4"/>
-      <c r="B107" s="6"/>
+      <c r="B107" s="7"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -4563,7 +4461,7 @@
     </row>
     <row r="108" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4"/>
-      <c r="B108" s="6"/>
+      <c r="B108" s="7"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -4576,7 +4474,7 @@
     </row>
     <row r="109" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="4"/>
-      <c r="B109" s="6"/>
+      <c r="B109" s="7"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -4589,7 +4487,7 @@
     </row>
     <row r="110" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="4"/>
-      <c r="B110" s="6"/>
+      <c r="B110" s="7"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -4602,7 +4500,7 @@
     </row>
     <row r="111" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="4"/>
-      <c r="B111" s="6"/>
+      <c r="B111" s="7"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -4615,7 +4513,7 @@
     </row>
     <row r="112" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="4"/>
-      <c r="B112" s="6"/>
+      <c r="B112" s="7"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -4628,7 +4526,7 @@
     </row>
     <row r="113" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="4"/>
-      <c r="B113" s="6"/>
+      <c r="B113" s="7"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -4641,7 +4539,7 @@
     </row>
     <row r="114" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="4"/>
-      <c r="B114" s="6"/>
+      <c r="B114" s="7"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -4654,7 +4552,7 @@
     </row>
     <row r="115" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="4"/>
-      <c r="B115" s="6"/>
+      <c r="B115" s="7"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -4667,7 +4565,7 @@
     </row>
     <row r="116" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="4"/>
-      <c r="B116" s="6"/>
+      <c r="B116" s="7"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -4680,7 +4578,7 @@
     </row>
     <row r="117" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="4"/>
-      <c r="B117" s="6"/>
+      <c r="B117" s="7"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -4693,7 +4591,7 @@
     </row>
     <row r="118" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="4"/>
-      <c r="B118" s="6"/>
+      <c r="B118" s="7"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -4706,7 +4604,7 @@
     </row>
     <row r="119" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="4"/>
-      <c r="B119" s="6"/>
+      <c r="B119" s="7"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -4719,7 +4617,7 @@
     </row>
     <row r="120" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="4"/>
-      <c r="B120" s="6"/>
+      <c r="B120" s="7"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -4732,7 +4630,7 @@
     </row>
     <row r="121" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="4"/>
-      <c r="B121" s="6"/>
+      <c r="B121" s="7"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -4745,7 +4643,7 @@
     </row>
     <row r="122" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="4"/>
-      <c r="B122" s="6"/>
+      <c r="B122" s="7"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -4758,7 +4656,7 @@
     </row>
     <row r="123" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="4"/>
-      <c r="B123" s="6"/>
+      <c r="B123" s="7"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -4771,7 +4669,7 @@
     </row>
     <row r="124" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="4"/>
-      <c r="B124" s="6"/>
+      <c r="B124" s="7"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
@@ -4784,7 +4682,7 @@
     </row>
     <row r="125" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="4"/>
-      <c r="B125" s="6"/>
+      <c r="B125" s="7"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -4797,7 +4695,7 @@
     </row>
     <row r="126" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="4"/>
-      <c r="B126" s="6"/>
+      <c r="B126" s="7"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -4810,7 +4708,7 @@
     </row>
     <row r="127" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="4"/>
-      <c r="B127" s="6"/>
+      <c r="B127" s="7"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -4823,7 +4721,7 @@
     </row>
     <row r="128" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="4"/>
-      <c r="B128" s="6"/>
+      <c r="B128" s="7"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -4836,7 +4734,7 @@
     </row>
     <row r="129" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="4"/>
-      <c r="B129" s="6"/>
+      <c r="B129" s="7"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -4849,7 +4747,7 @@
     </row>
     <row r="130" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="4"/>
-      <c r="B130" s="6"/>
+      <c r="B130" s="7"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -4862,7 +4760,7 @@
     </row>
     <row r="131" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="4"/>
-      <c r="B131" s="6"/>
+      <c r="B131" s="7"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -4875,7 +4773,7 @@
     </row>
     <row r="132" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="4"/>
-      <c r="B132" s="6"/>
+      <c r="B132" s="7"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -4888,7 +4786,7 @@
     </row>
     <row r="133" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="4"/>
-      <c r="B133" s="6"/>
+      <c r="B133" s="7"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -4901,7 +4799,7 @@
     </row>
     <row r="134" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="4"/>
-      <c r="B134" s="6"/>
+      <c r="B134" s="7"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
@@ -4914,7 +4812,7 @@
     </row>
     <row r="135" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="4"/>
-      <c r="B135" s="6"/>
+      <c r="B135" s="7"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
@@ -4927,7 +4825,7 @@
     </row>
     <row r="136" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="4"/>
-      <c r="B136" s="6"/>
+      <c r="B136" s="7"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
@@ -4940,7 +4838,7 @@
     </row>
     <row r="137" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="4"/>
-      <c r="B137" s="6"/>
+      <c r="B137" s="7"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -4953,7 +4851,7 @@
     </row>
     <row r="138" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="4"/>
-      <c r="B138" s="6"/>
+      <c r="B138" s="7"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
@@ -4966,7 +4864,7 @@
     </row>
     <row r="139" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="4"/>
-      <c r="B139" s="6"/>
+      <c r="B139" s="7"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -4979,7 +4877,7 @@
     </row>
     <row r="140" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="4"/>
-      <c r="B140" s="6"/>
+      <c r="B140" s="7"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -4992,7 +4890,7 @@
     </row>
     <row r="141" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="4"/>
-      <c r="B141" s="6"/>
+      <c r="B141" s="7"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
@@ -5005,7 +4903,7 @@
     </row>
     <row r="142" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="4"/>
-      <c r="B142" s="6"/>
+      <c r="B142" s="7"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
@@ -5018,7 +4916,7 @@
     </row>
     <row r="143" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="4"/>
-      <c r="B143" s="6"/>
+      <c r="B143" s="7"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
@@ -5031,7 +4929,7 @@
     </row>
     <row r="144" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="4"/>
-      <c r="B144" s="6"/>
+      <c r="B144" s="7"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -5044,7 +4942,7 @@
     </row>
     <row r="145" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="4"/>
-      <c r="B145" s="6"/>
+      <c r="B145" s="7"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
@@ -5057,7 +4955,7 @@
     </row>
     <row r="146" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="4"/>
-      <c r="B146" s="6"/>
+      <c r="B146" s="7"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -5070,7 +4968,7 @@
     </row>
     <row r="147" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="4"/>
-      <c r="B147" s="6"/>
+      <c r="B147" s="7"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
@@ -5083,7 +4981,7 @@
     </row>
     <row r="148" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="4"/>
-      <c r="B148" s="6"/>
+      <c r="B148" s="7"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
@@ -5096,7 +4994,7 @@
     </row>
     <row r="149" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="4"/>
-      <c r="B149" s="6"/>
+      <c r="B149" s="7"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -5109,7 +5007,7 @@
     </row>
     <row r="150" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="4"/>
-      <c r="B150" s="6"/>
+      <c r="B150" s="7"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
@@ -5122,7 +5020,7 @@
     </row>
     <row r="151" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="4"/>
-      <c r="B151" s="6"/>
+      <c r="B151" s="7"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
@@ -5135,7 +5033,7 @@
     </row>
     <row r="152" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="4"/>
-      <c r="B152" s="6"/>
+      <c r="B152" s="7"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -5148,7 +5046,7 @@
     </row>
     <row r="153" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="4"/>
-      <c r="B153" s="6"/>
+      <c r="B153" s="7"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
@@ -5161,7 +5059,7 @@
     </row>
     <row r="154" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="4"/>
-      <c r="B154" s="6"/>
+      <c r="B154" s="7"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
@@ -5174,7 +5072,7 @@
     </row>
     <row r="155" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="4"/>
-      <c r="B155" s="6"/>
+      <c r="B155" s="7"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
@@ -5187,7 +5085,7 @@
     </row>
     <row r="156" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="4"/>
-      <c r="B156" s="6"/>
+      <c r="B156" s="7"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
@@ -5200,7 +5098,7 @@
     </row>
     <row r="157" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="4"/>
-      <c r="B157" s="6"/>
+      <c r="B157" s="7"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
@@ -5213,7 +5111,7 @@
     </row>
     <row r="158" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="4"/>
-      <c r="B158" s="6"/>
+      <c r="B158" s="7"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -5226,7 +5124,7 @@
     </row>
     <row r="159" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="4"/>
-      <c r="B159" s="6"/>
+      <c r="B159" s="7"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
@@ -5239,7 +5137,7 @@
     </row>
     <row r="160" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="4"/>
-      <c r="B160" s="6"/>
+      <c r="B160" s="7"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
@@ -5252,7 +5150,7 @@
     </row>
     <row r="161" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="4"/>
-      <c r="B161" s="6"/>
+      <c r="B161" s="7"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -5265,7 +5163,7 @@
     </row>
     <row r="162" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="4"/>
-      <c r="B162" s="6"/>
+      <c r="B162" s="7"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
@@ -5278,7 +5176,7 @@
     </row>
     <row r="163" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="4"/>
-      <c r="B163" s="6"/>
+      <c r="B163" s="7"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
@@ -5291,7 +5189,7 @@
     </row>
     <row r="164" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="4"/>
-      <c r="B164" s="6"/>
+      <c r="B164" s="7"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
@@ -5304,7 +5202,7 @@
     </row>
     <row r="165" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="4"/>
-      <c r="B165" s="6"/>
+      <c r="B165" s="7"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
@@ -5317,7 +5215,7 @@
     </row>
     <row r="166" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="4"/>
-      <c r="B166" s="6"/>
+      <c r="B166" s="7"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
@@ -5330,7 +5228,7 @@
     </row>
     <row r="167" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="4"/>
-      <c r="B167" s="6"/>
+      <c r="B167" s="7"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
@@ -5343,7 +5241,7 @@
     </row>
     <row r="168" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="4"/>
-      <c r="B168" s="6"/>
+      <c r="B168" s="7"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
@@ -5356,7 +5254,7 @@
     </row>
     <row r="169" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="4"/>
-      <c r="B169" s="6"/>
+      <c r="B169" s="7"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
@@ -5369,7 +5267,7 @@
     </row>
     <row r="170" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="4"/>
-      <c r="B170" s="6"/>
+      <c r="B170" s="7"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -5382,7 +5280,7 @@
     </row>
     <row r="171" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="4"/>
-      <c r="B171" s="6"/>
+      <c r="B171" s="7"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
@@ -5395,7 +5293,7 @@
     </row>
     <row r="172" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="4"/>
-      <c r="B172" s="6"/>
+      <c r="B172" s="7"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
@@ -5408,7 +5306,7 @@
     </row>
     <row r="173" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="4"/>
-      <c r="B173" s="6"/>
+      <c r="B173" s="7"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
@@ -5421,7 +5319,7 @@
     </row>
     <row r="174" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="4"/>
-      <c r="B174" s="6"/>
+      <c r="B174" s="7"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
@@ -5434,7 +5332,7 @@
     </row>
     <row r="175" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="4"/>
-      <c r="B175" s="6"/>
+      <c r="B175" s="7"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
@@ -5447,7 +5345,7 @@
     </row>
     <row r="176" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="4"/>
-      <c r="B176" s="6"/>
+      <c r="B176" s="7"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
@@ -5460,7 +5358,7 @@
     </row>
     <row r="177" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="4"/>
-      <c r="B177" s="6"/>
+      <c r="B177" s="7"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
@@ -5473,7 +5371,7 @@
     </row>
     <row r="178" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="4"/>
-      <c r="B178" s="6"/>
+      <c r="B178" s="7"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
@@ -5486,7 +5384,7 @@
     </row>
     <row r="179" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A179" s="4"/>
-      <c r="B179" s="6"/>
+      <c r="B179" s="7"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
@@ -5499,7 +5397,7 @@
     </row>
     <row r="180" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="4"/>
-      <c r="B180" s="6"/>
+      <c r="B180" s="7"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
@@ -5512,7 +5410,7 @@
     </row>
     <row r="181" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="4"/>
-      <c r="B181" s="6"/>
+      <c r="B181" s="7"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
@@ -5525,7 +5423,7 @@
     </row>
     <row r="182" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="4"/>
-      <c r="B182" s="6"/>
+      <c r="B182" s="7"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
@@ -5538,7 +5436,7 @@
     </row>
     <row r="183" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="4"/>
-      <c r="B183" s="6"/>
+      <c r="B183" s="7"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
@@ -5551,7 +5449,7 @@
     </row>
     <row r="184" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="4"/>
-      <c r="B184" s="6"/>
+      <c r="B184" s="7"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
@@ -5564,7 +5462,7 @@
     </row>
     <row r="185" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="4"/>
-      <c r="B185" s="6"/>
+      <c r="B185" s="7"/>
       <c r="C185" s="4"/>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
@@ -5577,7 +5475,7 @@
     </row>
     <row r="186" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="4"/>
-      <c r="B186" s="6"/>
+      <c r="B186" s="7"/>
       <c r="C186" s="4"/>
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
@@ -5590,7 +5488,7 @@
     </row>
     <row r="187" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="4"/>
-      <c r="B187" s="6"/>
+      <c r="B187" s="7"/>
       <c r="C187" s="4"/>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
@@ -5603,7 +5501,7 @@
     </row>
     <row r="188" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="4"/>
-      <c r="B188" s="6"/>
+      <c r="B188" s="7"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
@@ -5616,7 +5514,7 @@
     </row>
     <row r="189" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="4"/>
-      <c r="B189" s="6"/>
+      <c r="B189" s="7"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
@@ -5629,7 +5527,7 @@
     </row>
     <row r="190" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="4"/>
-      <c r="B190" s="6"/>
+      <c r="B190" s="7"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
@@ -5642,7 +5540,7 @@
     </row>
     <row r="191" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A191" s="4"/>
-      <c r="B191" s="6"/>
+      <c r="B191" s="7"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
@@ -5655,7 +5553,7 @@
     </row>
     <row r="192" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A192" s="4"/>
-      <c r="B192" s="6"/>
+      <c r="B192" s="7"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
@@ -5668,7 +5566,7 @@
     </row>
     <row r="193" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A193" s="4"/>
-      <c r="B193" s="6"/>
+      <c r="B193" s="7"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
       <c r="E193" s="4"/>
@@ -5681,7 +5579,7 @@
     </row>
     <row r="194" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A194" s="4"/>
-      <c r="B194" s="6"/>
+      <c r="B194" s="7"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
@@ -5694,7 +5592,7 @@
     </row>
     <row r="195" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A195" s="4"/>
-      <c r="B195" s="6"/>
+      <c r="B195" s="7"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
@@ -5707,7 +5605,7 @@
     </row>
     <row r="196" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A196" s="4"/>
-      <c r="B196" s="6"/>
+      <c r="B196" s="7"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
@@ -5720,7 +5618,7 @@
     </row>
     <row r="197" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A197" s="4"/>
-      <c r="B197" s="6"/>
+      <c r="B197" s="7"/>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
@@ -5733,7 +5631,7 @@
     </row>
     <row r="198" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A198" s="4"/>
-      <c r="B198" s="6"/>
+      <c r="B198" s="7"/>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
       <c r="E198" s="4"/>
@@ -5746,7 +5644,7 @@
     </row>
     <row r="199" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A199" s="4"/>
-      <c r="B199" s="6"/>
+      <c r="B199" s="7"/>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
       <c r="E199" s="4"/>
@@ -5759,7 +5657,7 @@
     </row>
     <row r="200" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A200" s="4"/>
-      <c r="B200" s="6"/>
+      <c r="B200" s="7"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
       <c r="E200" s="4"/>
@@ -5772,7 +5670,7 @@
     </row>
     <row r="201" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A201" s="4"/>
-      <c r="B201" s="6"/>
+      <c r="B201" s="7"/>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
       <c r="E201" s="4"/>
@@ -5785,7 +5683,7 @@
     </row>
     <row r="202" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A202" s="4"/>
-      <c r="B202" s="6"/>
+      <c r="B202" s="7"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
       <c r="E202" s="4"/>
@@ -5798,7 +5696,7 @@
     </row>
     <row r="203" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A203" s="4"/>
-      <c r="B203" s="6"/>
+      <c r="B203" s="7"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
@@ -5811,7 +5709,7 @@
     </row>
     <row r="204" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A204" s="4"/>
-      <c r="B204" s="6"/>
+      <c r="B204" s="7"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
       <c r="E204" s="4"/>
@@ -5824,7 +5722,7 @@
     </row>
     <row r="205" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="4"/>
-      <c r="B205" s="6"/>
+      <c r="B205" s="7"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
       <c r="E205" s="4"/>
@@ -5837,7 +5735,7 @@
     </row>
     <row r="206" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="4"/>
-      <c r="B206" s="6"/>
+      <c r="B206" s="7"/>
       <c r="C206" s="4"/>
       <c r="D206" s="4"/>
       <c r="E206" s="4"/>
@@ -5850,7 +5748,7 @@
     </row>
     <row r="207" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A207" s="4"/>
-      <c r="B207" s="6"/>
+      <c r="B207" s="7"/>
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
       <c r="E207" s="4"/>
@@ -5863,7 +5761,7 @@
     </row>
     <row r="208" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A208" s="4"/>
-      <c r="B208" s="6"/>
+      <c r="B208" s="7"/>
       <c r="C208" s="4"/>
       <c r="D208" s="4"/>
       <c r="E208" s="4"/>
@@ -5876,7 +5774,7 @@
     </row>
     <row r="209" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A209" s="4"/>
-      <c r="B209" s="6"/>
+      <c r="B209" s="7"/>
       <c r="C209" s="4"/>
       <c r="D209" s="4"/>
       <c r="E209" s="4"/>
@@ -5889,7 +5787,7 @@
     </row>
     <row r="210" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A210" s="4"/>
-      <c r="B210" s="6"/>
+      <c r="B210" s="7"/>
       <c r="C210" s="4"/>
       <c r="D210" s="4"/>
       <c r="E210" s="4"/>
@@ -5902,7 +5800,7 @@
     </row>
     <row r="211" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A211" s="4"/>
-      <c r="B211" s="6"/>
+      <c r="B211" s="7"/>
       <c r="C211" s="4"/>
       <c r="D211" s="4"/>
       <c r="E211" s="4"/>
@@ -5915,7 +5813,7 @@
     </row>
     <row r="212" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A212" s="4"/>
-      <c r="B212" s="6"/>
+      <c r="B212" s="7"/>
       <c r="C212" s="4"/>
       <c r="D212" s="4"/>
       <c r="E212" s="4"/>
@@ -5928,7 +5826,7 @@
     </row>
     <row r="213" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A213" s="4"/>
-      <c r="B213" s="6"/>
+      <c r="B213" s="7"/>
       <c r="C213" s="4"/>
       <c r="D213" s="4"/>
       <c r="E213" s="4"/>
@@ -5941,7 +5839,7 @@
     </row>
     <row r="214" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A214" s="4"/>
-      <c r="B214" s="6"/>
+      <c r="B214" s="7"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
       <c r="E214" s="4"/>
@@ -5954,7 +5852,7 @@
     </row>
     <row r="215" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A215" s="4"/>
-      <c r="B215" s="6"/>
+      <c r="B215" s="7"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
       <c r="E215" s="4"/>
@@ -5967,7 +5865,7 @@
     </row>
     <row r="216" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A216" s="4"/>
-      <c r="B216" s="6"/>
+      <c r="B216" s="7"/>
       <c r="C216" s="4"/>
       <c r="D216" s="4"/>
       <c r="E216" s="4"/>
@@ -5980,7 +5878,7 @@
     </row>
     <row r="217" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A217" s="4"/>
-      <c r="B217" s="6"/>
+      <c r="B217" s="7"/>
       <c r="C217" s="4"/>
       <c r="D217" s="4"/>
       <c r="E217" s="4"/>
@@ -5993,7 +5891,7 @@
     </row>
     <row r="218" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A218" s="4"/>
-      <c r="B218" s="6"/>
+      <c r="B218" s="7"/>
       <c r="C218" s="4"/>
       <c r="D218" s="4"/>
       <c r="E218" s="4"/>
@@ -6006,7 +5904,7 @@
     </row>
     <row r="219" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A219" s="4"/>
-      <c r="B219" s="6"/>
+      <c r="B219" s="7"/>
       <c r="C219" s="4"/>
       <c r="D219" s="4"/>
       <c r="E219" s="4"/>
@@ -6019,7 +5917,7 @@
     </row>
     <row r="220" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A220" s="4"/>
-      <c r="B220" s="6"/>
+      <c r="B220" s="7"/>
       <c r="C220" s="4"/>
       <c r="D220" s="4"/>
       <c r="E220" s="4"/>
@@ -6032,7 +5930,7 @@
     </row>
     <row r="221" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A221" s="4"/>
-      <c r="B221" s="6"/>
+      <c r="B221" s="7"/>
       <c r="C221" s="4"/>
       <c r="D221" s="4"/>
       <c r="E221" s="4"/>
@@ -6045,7 +5943,7 @@
     </row>
     <row r="222" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A222" s="4"/>
-      <c r="B222" s="6"/>
+      <c r="B222" s="7"/>
       <c r="C222" s="4"/>
       <c r="D222" s="4"/>
       <c r="E222" s="4"/>
@@ -6058,7 +5956,7 @@
     </row>
     <row r="223" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A223" s="4"/>
-      <c r="B223" s="6"/>
+      <c r="B223" s="7"/>
       <c r="C223" s="4"/>
       <c r="D223" s="4"/>
       <c r="E223" s="4"/>
@@ -6071,7 +5969,7 @@
     </row>
     <row r="224" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A224" s="4"/>
-      <c r="B224" s="6"/>
+      <c r="B224" s="7"/>
       <c r="C224" s="4"/>
       <c r="D224" s="4"/>
       <c r="E224" s="4"/>
@@ -6084,7 +5982,7 @@
     </row>
     <row r="225" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="4"/>
-      <c r="B225" s="6"/>
+      <c r="B225" s="7"/>
       <c r="C225" s="4"/>
       <c r="D225" s="4"/>
       <c r="E225" s="4"/>
@@ -6097,7 +5995,7 @@
     </row>
     <row r="226" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="4"/>
-      <c r="B226" s="6"/>
+      <c r="B226" s="7"/>
       <c r="C226" s="4"/>
       <c r="D226" s="4"/>
       <c r="E226" s="4"/>
@@ -6110,7 +6008,7 @@
     </row>
     <row r="227" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="4"/>
-      <c r="B227" s="6"/>
+      <c r="B227" s="7"/>
       <c r="C227" s="4"/>
       <c r="D227" s="4"/>
       <c r="E227" s="4"/>
@@ -6123,7 +6021,7 @@
     </row>
     <row r="228" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="4"/>
-      <c r="B228" s="6"/>
+      <c r="B228" s="7"/>
       <c r="C228" s="4"/>
       <c r="D228" s="4"/>
       <c r="E228" s="4"/>
@@ -6136,7 +6034,7 @@
     </row>
     <row r="229" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="4"/>
-      <c r="B229" s="6"/>
+      <c r="B229" s="7"/>
       <c r="C229" s="4"/>
       <c r="D229" s="4"/>
       <c r="E229" s="4"/>
@@ -6149,7 +6047,7 @@
     </row>
     <row r="230" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="4"/>
-      <c r="B230" s="6"/>
+      <c r="B230" s="7"/>
       <c r="C230" s="4"/>
       <c r="D230" s="4"/>
       <c r="E230" s="4"/>
@@ -6162,7 +6060,7 @@
     </row>
     <row r="231" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="4"/>
-      <c r="B231" s="6"/>
+      <c r="B231" s="7"/>
       <c r="C231" s="4"/>
       <c r="D231" s="4"/>
       <c r="E231" s="4"/>
@@ -6175,7 +6073,7 @@
     </row>
     <row r="232" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="4"/>
-      <c r="B232" s="6"/>
+      <c r="B232" s="7"/>
       <c r="C232" s="4"/>
       <c r="D232" s="4"/>
       <c r="E232" s="4"/>
@@ -6188,7 +6086,7 @@
     </row>
     <row r="233" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="4"/>
-      <c r="B233" s="6"/>
+      <c r="B233" s="7"/>
       <c r="C233" s="4"/>
       <c r="D233" s="4"/>
       <c r="E233" s="4"/>
@@ -6201,7 +6099,7 @@
     </row>
     <row r="234" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="4"/>
-      <c r="B234" s="6"/>
+      <c r="B234" s="7"/>
       <c r="C234" s="4"/>
       <c r="D234" s="4"/>
       <c r="E234" s="4"/>
@@ -6214,7 +6112,7 @@
     </row>
     <row r="235" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="4"/>
-      <c r="B235" s="6"/>
+      <c r="B235" s="7"/>
       <c r="C235" s="4"/>
       <c r="D235" s="4"/>
       <c r="E235" s="4"/>
@@ -6227,7 +6125,7 @@
     </row>
     <row r="236" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="4"/>
-      <c r="B236" s="6"/>
+      <c r="B236" s="7"/>
       <c r="C236" s="4"/>
       <c r="D236" s="4"/>
       <c r="E236" s="4"/>
@@ -6240,7 +6138,7 @@
     </row>
     <row r="237" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="4"/>
-      <c r="B237" s="6"/>
+      <c r="B237" s="7"/>
       <c r="C237" s="4"/>
       <c r="D237" s="4"/>
       <c r="E237" s="4"/>
@@ -6253,7 +6151,7 @@
     </row>
     <row r="238" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="4"/>
-      <c r="B238" s="6"/>
+      <c r="B238" s="7"/>
       <c r="C238" s="4"/>
       <c r="D238" s="4"/>
       <c r="E238" s="4"/>
@@ -6266,7 +6164,7 @@
     </row>
     <row r="239" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="4"/>
-      <c r="B239" s="6"/>
+      <c r="B239" s="7"/>
       <c r="C239" s="4"/>
       <c r="D239" s="4"/>
       <c r="E239" s="4"/>
@@ -6279,7 +6177,7 @@
     </row>
     <row r="240" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="4"/>
-      <c r="B240" s="6"/>
+      <c r="B240" s="7"/>
       <c r="C240" s="4"/>
       <c r="D240" s="4"/>
       <c r="E240" s="4"/>
@@ -6292,7 +6190,7 @@
     </row>
     <row r="241" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="4"/>
-      <c r="B241" s="6"/>
+      <c r="B241" s="7"/>
       <c r="C241" s="4"/>
       <c r="D241" s="4"/>
       <c r="E241" s="4"/>
@@ -6305,7 +6203,7 @@
     </row>
     <row r="242" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A242" s="4"/>
-      <c r="B242" s="6"/>
+      <c r="B242" s="7"/>
       <c r="C242" s="4"/>
       <c r="D242" s="4"/>
       <c r="E242" s="4"/>
@@ -6318,7 +6216,7 @@
     </row>
     <row r="243" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A243" s="4"/>
-      <c r="B243" s="6"/>
+      <c r="B243" s="7"/>
       <c r="C243" s="4"/>
       <c r="D243" s="4"/>
       <c r="E243" s="4"/>
@@ -6331,7 +6229,7 @@
     </row>
     <row r="244" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A244" s="4"/>
-      <c r="B244" s="6"/>
+      <c r="B244" s="7"/>
       <c r="C244" s="4"/>
       <c r="D244" s="4"/>
       <c r="E244" s="4"/>
@@ -6344,7 +6242,7 @@
     </row>
     <row r="245" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="4"/>
-      <c r="B245" s="6"/>
+      <c r="B245" s="7"/>
       <c r="C245" s="4"/>
       <c r="D245" s="4"/>
       <c r="E245" s="4"/>
@@ -6357,7 +6255,7 @@
     </row>
     <row r="246" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="4"/>
-      <c r="B246" s="6"/>
+      <c r="B246" s="7"/>
       <c r="C246" s="4"/>
       <c r="D246" s="4"/>
       <c r="E246" s="4"/>
@@ -6370,7 +6268,7 @@
     </row>
     <row r="247" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A247" s="4"/>
-      <c r="B247" s="6"/>
+      <c r="B247" s="7"/>
       <c r="C247" s="4"/>
       <c r="D247" s="4"/>
       <c r="E247" s="4"/>
@@ -6383,7 +6281,7 @@
     </row>
     <row r="248" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A248" s="4"/>
-      <c r="B248" s="6"/>
+      <c r="B248" s="7"/>
       <c r="C248" s="4"/>
       <c r="D248" s="4"/>
       <c r="E248" s="4"/>
@@ -6396,7 +6294,7 @@
     </row>
     <row r="249" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A249" s="4"/>
-      <c r="B249" s="6"/>
+      <c r="B249" s="7"/>
       <c r="C249" s="4"/>
       <c r="D249" s="4"/>
       <c r="E249" s="4"/>
@@ -6409,7 +6307,7 @@
     </row>
     <row r="250" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A250" s="4"/>
-      <c r="B250" s="6"/>
+      <c r="B250" s="7"/>
       <c r="C250" s="4"/>
       <c r="D250" s="4"/>
       <c r="E250" s="4"/>
@@ -6422,7 +6320,7 @@
     </row>
     <row r="251" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A251" s="4"/>
-      <c r="B251" s="6"/>
+      <c r="B251" s="7"/>
       <c r="C251" s="4"/>
       <c r="D251" s="4"/>
       <c r="E251" s="4"/>
@@ -6435,7 +6333,7 @@
     </row>
     <row r="252" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A252" s="4"/>
-      <c r="B252" s="6"/>
+      <c r="B252" s="7"/>
       <c r="C252" s="4"/>
       <c r="D252" s="4"/>
       <c r="E252" s="4"/>
@@ -6448,7 +6346,7 @@
     </row>
     <row r="253" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A253" s="4"/>
-      <c r="B253" s="6"/>
+      <c r="B253" s="7"/>
       <c r="C253" s="4"/>
       <c r="D253" s="4"/>
       <c r="E253" s="4"/>
@@ -6461,7 +6359,7 @@
     </row>
     <row r="254" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A254" s="4"/>
-      <c r="B254" s="6"/>
+      <c r="B254" s="7"/>
       <c r="C254" s="4"/>
       <c r="D254" s="4"/>
       <c r="E254" s="4"/>
@@ -6474,7 +6372,7 @@
     </row>
     <row r="255" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A255" s="4"/>
-      <c r="B255" s="6"/>
+      <c r="B255" s="7"/>
       <c r="C255" s="4"/>
       <c r="D255" s="4"/>
       <c r="E255" s="4"/>
@@ -6487,7 +6385,7 @@
     </row>
     <row r="256" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A256" s="4"/>
-      <c r="B256" s="6"/>
+      <c r="B256" s="7"/>
       <c r="C256" s="4"/>
       <c r="D256" s="4"/>
       <c r="E256" s="4"/>
@@ -6500,7 +6398,7 @@
     </row>
     <row r="257" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A257" s="4"/>
-      <c r="B257" s="6"/>
+      <c r="B257" s="7"/>
       <c r="C257" s="4"/>
       <c r="D257" s="4"/>
       <c r="E257" s="4"/>
@@ -6513,7 +6411,7 @@
     </row>
     <row r="258" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A258" s="4"/>
-      <c r="B258" s="6"/>
+      <c r="B258" s="7"/>
       <c r="C258" s="4"/>
       <c r="D258" s="4"/>
       <c r="E258" s="4"/>
@@ -6526,7 +6424,7 @@
     </row>
     <row r="259" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A259" s="4"/>
-      <c r="B259" s="6"/>
+      <c r="B259" s="7"/>
       <c r="C259" s="4"/>
       <c r="D259" s="4"/>
       <c r="E259" s="4"/>
@@ -6539,7 +6437,7 @@
     </row>
     <row r="260" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A260" s="4"/>
-      <c r="B260" s="6"/>
+      <c r="B260" s="7"/>
       <c r="C260" s="4"/>
       <c r="D260" s="4"/>
       <c r="E260" s="4"/>
@@ -6552,7 +6450,7 @@
     </row>
     <row r="261" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A261" s="4"/>
-      <c r="B261" s="6"/>
+      <c r="B261" s="7"/>
       <c r="C261" s="4"/>
       <c r="D261" s="4"/>
       <c r="E261" s="4"/>
@@ -6565,7 +6463,7 @@
     </row>
     <row r="262" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A262" s="4"/>
-      <c r="B262" s="6"/>
+      <c r="B262" s="7"/>
       <c r="C262" s="4"/>
       <c r="D262" s="4"/>
       <c r="E262" s="4"/>
@@ -6578,7 +6476,7 @@
     </row>
     <row r="263" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A263" s="4"/>
-      <c r="B263" s="6"/>
+      <c r="B263" s="7"/>
       <c r="C263" s="4"/>
       <c r="D263" s="4"/>
       <c r="E263" s="4"/>
@@ -6591,7 +6489,7 @@
     </row>
     <row r="264" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A264" s="4"/>
-      <c r="B264" s="6"/>
+      <c r="B264" s="7"/>
       <c r="C264" s="4"/>
       <c r="D264" s="4"/>
       <c r="E264" s="4"/>
@@ -6604,7 +6502,7 @@
     </row>
     <row r="265" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A265" s="4"/>
-      <c r="B265" s="6"/>
+      <c r="B265" s="7"/>
       <c r="C265" s="4"/>
       <c r="D265" s="4"/>
       <c r="E265" s="4"/>
@@ -6617,7 +6515,7 @@
     </row>
     <row r="266" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A266" s="4"/>
-      <c r="B266" s="6"/>
+      <c r="B266" s="7"/>
       <c r="C266" s="4"/>
       <c r="D266" s="4"/>
       <c r="E266" s="4"/>
@@ -6630,7 +6528,7 @@
     </row>
     <row r="267" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A267" s="4"/>
-      <c r="B267" s="6"/>
+      <c r="B267" s="7"/>
       <c r="C267" s="4"/>
       <c r="D267" s="4"/>
       <c r="E267" s="4"/>
@@ -6643,7 +6541,7 @@
     </row>
     <row r="268" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A268" s="4"/>
-      <c r="B268" s="6"/>
+      <c r="B268" s="7"/>
       <c r="C268" s="4"/>
       <c r="D268" s="4"/>
       <c r="E268" s="4"/>
@@ -6656,7 +6554,7 @@
     </row>
     <row r="269" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A269" s="4"/>
-      <c r="B269" s="6"/>
+      <c r="B269" s="7"/>
       <c r="C269" s="4"/>
       <c r="D269" s="4"/>
       <c r="E269" s="4"/>
@@ -6669,7 +6567,7 @@
     </row>
     <row r="270" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A270" s="4"/>
-      <c r="B270" s="6"/>
+      <c r="B270" s="7"/>
       <c r="C270" s="4"/>
       <c r="D270" s="4"/>
       <c r="E270" s="4"/>
@@ -6682,7 +6580,7 @@
     </row>
     <row r="271" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A271" s="4"/>
-      <c r="B271" s="6"/>
+      <c r="B271" s="7"/>
       <c r="C271" s="4"/>
       <c r="D271" s="4"/>
       <c r="E271" s="4"/>
@@ -6695,7 +6593,7 @@
     </row>
     <row r="272" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A272" s="4"/>
-      <c r="B272" s="6"/>
+      <c r="B272" s="7"/>
       <c r="C272" s="4"/>
       <c r="D272" s="4"/>
       <c r="E272" s="4"/>
@@ -6708,7 +6606,7 @@
     </row>
     <row r="273" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A273" s="4"/>
-      <c r="B273" s="6"/>
+      <c r="B273" s="7"/>
       <c r="C273" s="4"/>
       <c r="D273" s="4"/>
       <c r="E273" s="4"/>
@@ -6721,7 +6619,7 @@
     </row>
     <row r="274" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="4"/>
-      <c r="B274" s="6"/>
+      <c r="B274" s="7"/>
       <c r="C274" s="4"/>
       <c r="D274" s="4"/>
       <c r="E274" s="4"/>
@@ -6734,7 +6632,7 @@
     </row>
     <row r="275" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A275" s="4"/>
-      <c r="B275" s="6"/>
+      <c r="B275" s="7"/>
       <c r="C275" s="4"/>
       <c r="D275" s="4"/>
       <c r="E275" s="4"/>
@@ -6747,7 +6645,7 @@
     </row>
     <row r="276" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A276" s="4"/>
-      <c r="B276" s="6"/>
+      <c r="B276" s="7"/>
       <c r="C276" s="4"/>
       <c r="D276" s="4"/>
       <c r="E276" s="4"/>
@@ -6760,7 +6658,7 @@
     </row>
     <row r="277" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A277" s="4"/>
-      <c r="B277" s="6"/>
+      <c r="B277" s="7"/>
       <c r="C277" s="4"/>
       <c r="D277" s="4"/>
       <c r="E277" s="4"/>
@@ -6773,7 +6671,7 @@
     </row>
     <row r="278" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A278" s="4"/>
-      <c r="B278" s="6"/>
+      <c r="B278" s="7"/>
       <c r="C278" s="4"/>
       <c r="D278" s="4"/>
       <c r="E278" s="4"/>
@@ -6786,7 +6684,7 @@
     </row>
     <row r="279" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A279" s="4"/>
-      <c r="B279" s="6"/>
+      <c r="B279" s="7"/>
       <c r="C279" s="4"/>
       <c r="D279" s="4"/>
       <c r="E279" s="4"/>
@@ -6799,7 +6697,7 @@
     </row>
     <row r="280" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A280" s="4"/>
-      <c r="B280" s="6"/>
+      <c r="B280" s="7"/>
       <c r="C280" s="4"/>
       <c r="D280" s="4"/>
       <c r="E280" s="4"/>
@@ -6812,7 +6710,7 @@
     </row>
     <row r="281" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A281" s="4"/>
-      <c r="B281" s="6"/>
+      <c r="B281" s="7"/>
       <c r="C281" s="4"/>
       <c r="D281" s="4"/>
       <c r="E281" s="4"/>
@@ -6825,7 +6723,7 @@
     </row>
     <row r="282" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A282" s="4"/>
-      <c r="B282" s="6"/>
+      <c r="B282" s="7"/>
       <c r="C282" s="4"/>
       <c r="D282" s="4"/>
       <c r="E282" s="4"/>
@@ -6838,7 +6736,7 @@
     </row>
     <row r="283" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A283" s="4"/>
-      <c r="B283" s="6"/>
+      <c r="B283" s="7"/>
       <c r="C283" s="4"/>
       <c r="D283" s="4"/>
       <c r="E283" s="4"/>
@@ -6851,7 +6749,7 @@
     </row>
     <row r="284" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A284" s="4"/>
-      <c r="B284" s="6"/>
+      <c r="B284" s="7"/>
       <c r="C284" s="4"/>
       <c r="D284" s="4"/>
       <c r="E284" s="4"/>
@@ -6864,7 +6762,7 @@
     </row>
     <row r="285" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A285" s="4"/>
-      <c r="B285" s="6"/>
+      <c r="B285" s="7"/>
       <c r="C285" s="4"/>
       <c r="D285" s="4"/>
       <c r="E285" s="4"/>
@@ -6877,7 +6775,7 @@
     </row>
     <row r="286" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A286" s="4"/>
-      <c r="B286" s="6"/>
+      <c r="B286" s="7"/>
       <c r="C286" s="4"/>
       <c r="D286" s="4"/>
       <c r="E286" s="4"/>
@@ -6890,7 +6788,7 @@
     </row>
     <row r="287" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A287" s="4"/>
-      <c r="B287" s="6"/>
+      <c r="B287" s="7"/>
       <c r="C287" s="4"/>
       <c r="D287" s="4"/>
       <c r="E287" s="4"/>
@@ -6903,7 +6801,7 @@
     </row>
     <row r="288" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A288" s="4"/>
-      <c r="B288" s="6"/>
+      <c r="B288" s="7"/>
       <c r="C288" s="4"/>
       <c r="D288" s="4"/>
       <c r="E288" s="4"/>
@@ -6916,7 +6814,7 @@
     </row>
     <row r="289" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A289" s="4"/>
-      <c r="B289" s="6"/>
+      <c r="B289" s="7"/>
       <c r="C289" s="4"/>
       <c r="D289" s="4"/>
       <c r="E289" s="4"/>
@@ -6929,7 +6827,7 @@
     </row>
     <row r="290" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A290" s="4"/>
-      <c r="B290" s="6"/>
+      <c r="B290" s="7"/>
       <c r="C290" s="4"/>
       <c r="D290" s="4"/>
       <c r="E290" s="4"/>
@@ -6942,7 +6840,7 @@
     </row>
     <row r="291" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A291" s="4"/>
-      <c r="B291" s="6"/>
+      <c r="B291" s="7"/>
       <c r="C291" s="4"/>
       <c r="D291" s="4"/>
       <c r="E291" s="4"/>
@@ -6955,7 +6853,7 @@
     </row>
     <row r="292" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A292" s="4"/>
-      <c r="B292" s="6"/>
+      <c r="B292" s="7"/>
       <c r="C292" s="4"/>
       <c r="D292" s="4"/>
       <c r="E292" s="4"/>
@@ -6968,7 +6866,7 @@
     </row>
     <row r="293" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A293" s="4"/>
-      <c r="B293" s="6"/>
+      <c r="B293" s="7"/>
       <c r="C293" s="4"/>
       <c r="D293" s="4"/>
       <c r="E293" s="4"/>
@@ -6981,7 +6879,7 @@
     </row>
     <row r="294" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A294" s="4"/>
-      <c r="B294" s="6"/>
+      <c r="B294" s="7"/>
       <c r="C294" s="4"/>
       <c r="D294" s="4"/>
       <c r="E294" s="4"/>
@@ -6994,7 +6892,7 @@
     </row>
     <row r="295" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A295" s="4"/>
-      <c r="B295" s="6"/>
+      <c r="B295" s="7"/>
       <c r="C295" s="4"/>
       <c r="D295" s="4"/>
       <c r="E295" s="4"/>
@@ -7007,7 +6905,7 @@
     </row>
     <row r="296" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A296" s="4"/>
-      <c r="B296" s="6"/>
+      <c r="B296" s="7"/>
       <c r="C296" s="4"/>
       <c r="D296" s="4"/>
       <c r="E296" s="4"/>
@@ -7020,7 +6918,7 @@
     </row>
     <row r="297" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A297" s="4"/>
-      <c r="B297" s="6"/>
+      <c r="B297" s="7"/>
       <c r="C297" s="4"/>
       <c r="D297" s="4"/>
       <c r="E297" s="4"/>
@@ -7033,7 +6931,7 @@
     </row>
     <row r="298" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A298" s="4"/>
-      <c r="B298" s="6"/>
+      <c r="B298" s="7"/>
       <c r="C298" s="4"/>
       <c r="D298" s="4"/>
       <c r="E298" s="4"/>
@@ -7046,7 +6944,7 @@
     </row>
     <row r="299" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A299" s="4"/>
-      <c r="B299" s="6"/>
+      <c r="B299" s="7"/>
       <c r="C299" s="4"/>
       <c r="D299" s="4"/>
       <c r="E299" s="4"/>
@@ -7059,7 +6957,7 @@
     </row>
     <row r="300" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A300" s="4"/>
-      <c r="B300" s="6"/>
+      <c r="B300" s="7"/>
       <c r="C300" s="4"/>
       <c r="D300" s="4"/>
       <c r="E300" s="4"/>
@@ -7072,7 +6970,7 @@
     </row>
     <row r="301" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A301" s="4"/>
-      <c r="B301" s="6"/>
+      <c r="B301" s="7"/>
       <c r="C301" s="4"/>
       <c r="D301" s="4"/>
       <c r="E301" s="4"/>
@@ -7085,7 +6983,7 @@
     </row>
     <row r="302" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A302" s="4"/>
-      <c r="B302" s="6"/>
+      <c r="B302" s="7"/>
       <c r="C302" s="4"/>
       <c r="D302" s="4"/>
       <c r="E302" s="4"/>
@@ -7098,7 +6996,7 @@
     </row>
     <row r="303" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A303" s="4"/>
-      <c r="B303" s="6"/>
+      <c r="B303" s="7"/>
       <c r="C303" s="4"/>
       <c r="D303" s="4"/>
       <c r="E303" s="4"/>
@@ -7111,7 +7009,7 @@
     </row>
     <row r="304" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A304" s="4"/>
-      <c r="B304" s="6"/>
+      <c r="B304" s="7"/>
       <c r="C304" s="4"/>
       <c r="D304" s="4"/>
       <c r="E304" s="4"/>
@@ -7124,7 +7022,7 @@
     </row>
     <row r="305" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A305" s="4"/>
-      <c r="B305" s="6"/>
+      <c r="B305" s="7"/>
       <c r="C305" s="4"/>
       <c r="D305" s="4"/>
       <c r="E305" s="4"/>
@@ -7137,7 +7035,7 @@
     </row>
     <row r="306" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A306" s="4"/>
-      <c r="B306" s="6"/>
+      <c r="B306" s="7"/>
       <c r="C306" s="4"/>
       <c r="D306" s="4"/>
       <c r="E306" s="4"/>
@@ -7150,7 +7048,7 @@
     </row>
     <row r="307" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A307" s="4"/>
-      <c r="B307" s="6"/>
+      <c r="B307" s="7"/>
       <c r="C307" s="4"/>
       <c r="D307" s="4"/>
       <c r="E307" s="4"/>
@@ -7163,7 +7061,7 @@
     </row>
     <row r="308" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A308" s="4"/>
-      <c r="B308" s="6"/>
+      <c r="B308" s="7"/>
       <c r="C308" s="4"/>
       <c r="D308" s="4"/>
       <c r="E308" s="4"/>
@@ -7176,7 +7074,7 @@
     </row>
     <row r="309" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A309" s="4"/>
-      <c r="B309" s="6"/>
+      <c r="B309" s="7"/>
       <c r="C309" s="4"/>
       <c r="D309" s="4"/>
       <c r="E309" s="4"/>
@@ -7189,7 +7087,7 @@
     </row>
     <row r="310" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A310" s="4"/>
-      <c r="B310" s="6"/>
+      <c r="B310" s="7"/>
       <c r="C310" s="4"/>
       <c r="D310" s="4"/>
       <c r="E310" s="4"/>
@@ -7202,7 +7100,7 @@
     </row>
     <row r="311" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A311" s="4"/>
-      <c r="B311" s="6"/>
+      <c r="B311" s="7"/>
       <c r="C311" s="4"/>
       <c r="D311" s="4"/>
       <c r="E311" s="4"/>
@@ -7215,7 +7113,7 @@
     </row>
     <row r="312" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A312" s="4"/>
-      <c r="B312" s="6"/>
+      <c r="B312" s="7"/>
       <c r="C312" s="4"/>
       <c r="D312" s="4"/>
       <c r="E312" s="4"/>
@@ -7228,7 +7126,7 @@
     </row>
     <row r="313" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A313" s="4"/>
-      <c r="B313" s="6"/>
+      <c r="B313" s="7"/>
       <c r="C313" s="4"/>
       <c r="D313" s="4"/>
       <c r="E313" s="4"/>
@@ -7241,7 +7139,7 @@
     </row>
     <row r="314" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A314" s="4"/>
-      <c r="B314" s="6"/>
+      <c r="B314" s="7"/>
       <c r="C314" s="4"/>
       <c r="D314" s="4"/>
       <c r="E314" s="4"/>
@@ -7254,7 +7152,7 @@
     </row>
     <row r="315" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A315" s="4"/>
-      <c r="B315" s="6"/>
+      <c r="B315" s="7"/>
       <c r="C315" s="4"/>
       <c r="D315" s="4"/>
       <c r="E315" s="4"/>
@@ -7267,7 +7165,7 @@
     </row>
     <row r="316" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A316" s="4"/>
-      <c r="B316" s="6"/>
+      <c r="B316" s="7"/>
       <c r="C316" s="4"/>
       <c r="D316" s="4"/>
       <c r="E316" s="4"/>
@@ -7280,7 +7178,7 @@
     </row>
     <row r="317" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A317" s="4"/>
-      <c r="B317" s="6"/>
+      <c r="B317" s="7"/>
       <c r="C317" s="4"/>
       <c r="D317" s="4"/>
       <c r="E317" s="4"/>
@@ -7293,7 +7191,7 @@
     </row>
     <row r="318" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A318" s="4"/>
-      <c r="B318" s="6"/>
+      <c r="B318" s="7"/>
       <c r="C318" s="4"/>
       <c r="D318" s="4"/>
       <c r="E318" s="4"/>
@@ -7306,7 +7204,7 @@
     </row>
     <row r="319" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A319" s="4"/>
-      <c r="B319" s="6"/>
+      <c r="B319" s="7"/>
       <c r="C319" s="4"/>
       <c r="D319" s="4"/>
       <c r="E319" s="4"/>
@@ -7319,7 +7217,7 @@
     </row>
     <row r="320" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A320" s="4"/>
-      <c r="B320" s="6"/>
+      <c r="B320" s="7"/>
       <c r="C320" s="4"/>
       <c r="D320" s="4"/>
       <c r="E320" s="4"/>
@@ -7332,7 +7230,7 @@
     </row>
     <row r="321" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A321" s="4"/>
-      <c r="B321" s="6"/>
+      <c r="B321" s="7"/>
       <c r="C321" s="4"/>
       <c r="D321" s="4"/>
       <c r="E321" s="4"/>
@@ -7345,7 +7243,7 @@
     </row>
     <row r="322" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A322" s="4"/>
-      <c r="B322" s="6"/>
+      <c r="B322" s="7"/>
       <c r="C322" s="4"/>
       <c r="D322" s="4"/>
       <c r="E322" s="4"/>
@@ -7358,7 +7256,7 @@
     </row>
     <row r="323" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A323" s="4"/>
-      <c r="B323" s="6"/>
+      <c r="B323" s="7"/>
       <c r="C323" s="4"/>
       <c r="D323" s="4"/>
       <c r="E323" s="4"/>
@@ -7371,7 +7269,7 @@
     </row>
     <row r="324" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A324" s="4"/>
-      <c r="B324" s="6"/>
+      <c r="B324" s="7"/>
       <c r="C324" s="4"/>
       <c r="D324" s="4"/>
       <c r="E324" s="4"/>
@@ -7384,7 +7282,7 @@
     </row>
     <row r="325" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A325" s="4"/>
-      <c r="B325" s="6"/>
+      <c r="B325" s="7"/>
       <c r="C325" s="4"/>
       <c r="D325" s="4"/>
       <c r="E325" s="4"/>
@@ -7397,7 +7295,7 @@
     </row>
     <row r="326" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A326" s="4"/>
-      <c r="B326" s="6"/>
+      <c r="B326" s="7"/>
       <c r="C326" s="4"/>
       <c r="D326" s="4"/>
       <c r="E326" s="4"/>
@@ -7410,7 +7308,7 @@
     </row>
     <row r="327" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A327" s="4"/>
-      <c r="B327" s="6"/>
+      <c r="B327" s="7"/>
       <c r="C327" s="4"/>
       <c r="D327" s="4"/>
       <c r="E327" s="4"/>
@@ -7423,7 +7321,7 @@
     </row>
     <row r="328" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A328" s="4"/>
-      <c r="B328" s="6"/>
+      <c r="B328" s="7"/>
       <c r="C328" s="4"/>
       <c r="D328" s="4"/>
       <c r="E328" s="4"/>
@@ -7436,7 +7334,7 @@
     </row>
     <row r="329" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A329" s="4"/>
-      <c r="B329" s="6"/>
+      <c r="B329" s="7"/>
       <c r="C329" s="4"/>
       <c r="D329" s="4"/>
       <c r="E329" s="4"/>
@@ -7449,7 +7347,7 @@
     </row>
     <row r="330" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A330" s="4"/>
-      <c r="B330" s="6"/>
+      <c r="B330" s="7"/>
       <c r="C330" s="4"/>
       <c r="D330" s="4"/>
       <c r="E330" s="4"/>
@@ -7462,7 +7360,7 @@
     </row>
     <row r="331" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A331" s="4"/>
-      <c r="B331" s="6"/>
+      <c r="B331" s="7"/>
       <c r="C331" s="4"/>
       <c r="D331" s="4"/>
       <c r="E331" s="4"/>
@@ -7475,7 +7373,7 @@
     </row>
     <row r="332" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A332" s="4"/>
-      <c r="B332" s="6"/>
+      <c r="B332" s="7"/>
       <c r="C332" s="4"/>
       <c r="D332" s="4"/>
       <c r="E332" s="4"/>
@@ -7488,7 +7386,7 @@
     </row>
     <row r="333" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A333" s="4"/>
-      <c r="B333" s="6"/>
+      <c r="B333" s="7"/>
       <c r="C333" s="4"/>
       <c r="D333" s="4"/>
       <c r="E333" s="4"/>
@@ -7501,7 +7399,7 @@
     </row>
     <row r="334" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A334" s="4"/>
-      <c r="B334" s="6"/>
+      <c r="B334" s="7"/>
       <c r="C334" s="4"/>
       <c r="D334" s="4"/>
       <c r="E334" s="4"/>
@@ -7514,7 +7412,7 @@
     </row>
     <row r="335" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A335" s="4"/>
-      <c r="B335" s="6"/>
+      <c r="B335" s="7"/>
       <c r="C335" s="4"/>
       <c r="D335" s="4"/>
       <c r="E335" s="4"/>
@@ -7527,7 +7425,7 @@
     </row>
     <row r="336" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A336" s="4"/>
-      <c r="B336" s="6"/>
+      <c r="B336" s="7"/>
       <c r="C336" s="4"/>
       <c r="D336" s="4"/>
       <c r="E336" s="4"/>
@@ -7540,7 +7438,7 @@
     </row>
     <row r="337" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A337" s="4"/>
-      <c r="B337" s="6"/>
+      <c r="B337" s="7"/>
       <c r="C337" s="4"/>
       <c r="D337" s="4"/>
       <c r="E337" s="4"/>
@@ -7553,7 +7451,7 @@
     </row>
     <row r="338" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A338" s="4"/>
-      <c r="B338" s="6"/>
+      <c r="B338" s="7"/>
       <c r="C338" s="4"/>
       <c r="D338" s="4"/>
       <c r="E338" s="4"/>
@@ -7566,7 +7464,7 @@
     </row>
     <row r="339" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A339" s="4"/>
-      <c r="B339" s="6"/>
+      <c r="B339" s="7"/>
       <c r="C339" s="4"/>
       <c r="D339" s="4"/>
       <c r="E339" s="4"/>
@@ -7579,7 +7477,7 @@
     </row>
     <row r="340" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A340" s="4"/>
-      <c r="B340" s="6"/>
+      <c r="B340" s="7"/>
       <c r="C340" s="4"/>
       <c r="D340" s="4"/>
       <c r="E340" s="4"/>
@@ -7592,7 +7490,7 @@
     </row>
     <row r="341" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A341" s="4"/>
-      <c r="B341" s="6"/>
+      <c r="B341" s="7"/>
       <c r="C341" s="4"/>
       <c r="D341" s="4"/>
       <c r="E341" s="4"/>
@@ -7605,7 +7503,7 @@
     </row>
     <row r="342" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A342" s="4"/>
-      <c r="B342" s="6"/>
+      <c r="B342" s="7"/>
       <c r="C342" s="4"/>
       <c r="D342" s="4"/>
       <c r="E342" s="4"/>
@@ -7618,7 +7516,7 @@
     </row>
     <row r="343" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A343" s="4"/>
-      <c r="B343" s="6"/>
+      <c r="B343" s="7"/>
       <c r="C343" s="4"/>
       <c r="D343" s="4"/>
       <c r="E343" s="4"/>
@@ -7631,7 +7529,7 @@
     </row>
     <row r="344" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="4"/>
-      <c r="B344" s="6"/>
+      <c r="B344" s="7"/>
       <c r="C344" s="4"/>
       <c r="D344" s="4"/>
       <c r="E344" s="4"/>
@@ -7644,7 +7542,7 @@
     </row>
     <row r="345" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A345" s="4"/>
-      <c r="B345" s="6"/>
+      <c r="B345" s="7"/>
       <c r="C345" s="4"/>
       <c r="D345" s="4"/>
       <c r="E345" s="4"/>
@@ -7657,7 +7555,7 @@
     </row>
     <row r="346" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A346" s="4"/>
-      <c r="B346" s="6"/>
+      <c r="B346" s="7"/>
       <c r="C346" s="4"/>
       <c r="D346" s="4"/>
       <c r="E346" s="4"/>
@@ -7670,7 +7568,7 @@
     </row>
     <row r="347" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A347" s="4"/>
-      <c r="B347" s="6"/>
+      <c r="B347" s="7"/>
       <c r="C347" s="4"/>
       <c r="D347" s="4"/>
       <c r="E347" s="4"/>
@@ -7683,7 +7581,7 @@
     </row>
     <row r="348" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A348" s="4"/>
-      <c r="B348" s="6"/>
+      <c r="B348" s="7"/>
       <c r="C348" s="4"/>
       <c r="D348" s="4"/>
       <c r="E348" s="4"/>
@@ -7696,7 +7594,7 @@
     </row>
     <row r="349" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A349" s="4"/>
-      <c r="B349" s="6"/>
+      <c r="B349" s="7"/>
       <c r="C349" s="4"/>
       <c r="D349" s="4"/>
       <c r="E349" s="4"/>
@@ -7709,7 +7607,7 @@
     </row>
     <row r="350" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="4"/>
-      <c r="B350" s="6"/>
+      <c r="B350" s="7"/>
       <c r="C350" s="4"/>
       <c r="D350" s="4"/>
       <c r="E350" s="4"/>
@@ -7722,7 +7620,7 @@
     </row>
     <row r="351" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="4"/>
-      <c r="B351" s="6"/>
+      <c r="B351" s="7"/>
       <c r="C351" s="4"/>
       <c r="D351" s="4"/>
       <c r="E351" s="4"/>
@@ -7735,7 +7633,7 @@
     </row>
     <row r="352" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A352" s="4"/>
-      <c r="B352" s="6"/>
+      <c r="B352" s="7"/>
       <c r="C352" s="4"/>
       <c r="D352" s="4"/>
       <c r="E352" s="4"/>
@@ -7748,7 +7646,7 @@
     </row>
     <row r="353" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A353" s="4"/>
-      <c r="B353" s="6"/>
+      <c r="B353" s="7"/>
       <c r="C353" s="4"/>
       <c r="D353" s="4"/>
       <c r="E353" s="4"/>
@@ -7761,7 +7659,7 @@
     </row>
     <row r="354" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A354" s="4"/>
-      <c r="B354" s="6"/>
+      <c r="B354" s="7"/>
       <c r="C354" s="4"/>
       <c r="D354" s="4"/>
       <c r="E354" s="4"/>
@@ -7774,7 +7672,7 @@
     </row>
     <row r="355" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A355" s="4"/>
-      <c r="B355" s="6"/>
+      <c r="B355" s="7"/>
       <c r="C355" s="4"/>
       <c r="D355" s="4"/>
       <c r="E355" s="4"/>
@@ -7787,7 +7685,7 @@
     </row>
     <row r="356" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A356" s="4"/>
-      <c r="B356" s="6"/>
+      <c r="B356" s="7"/>
       <c r="C356" s="4"/>
       <c r="D356" s="4"/>
       <c r="E356" s="4"/>
@@ -7800,7 +7698,7 @@
     </row>
     <row r="357" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A357" s="4"/>
-      <c r="B357" s="6"/>
+      <c r="B357" s="7"/>
       <c r="C357" s="4"/>
       <c r="D357" s="4"/>
       <c r="E357" s="4"/>
@@ -7813,7 +7711,7 @@
     </row>
     <row r="358" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A358" s="4"/>
-      <c r="B358" s="6"/>
+      <c r="B358" s="7"/>
       <c r="C358" s="4"/>
       <c r="D358" s="4"/>
       <c r="E358" s="4"/>
@@ -7826,7 +7724,7 @@
     </row>
     <row r="359" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A359" s="4"/>
-      <c r="B359" s="6"/>
+      <c r="B359" s="7"/>
       <c r="C359" s="4"/>
       <c r="D359" s="4"/>
       <c r="E359" s="4"/>
@@ -7839,7 +7737,7 @@
     </row>
     <row r="360" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A360" s="4"/>
-      <c r="B360" s="6"/>
+      <c r="B360" s="7"/>
       <c r="C360" s="4"/>
       <c r="D360" s="4"/>
       <c r="E360" s="4"/>
@@ -7852,7 +7750,7 @@
     </row>
     <row r="361" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A361" s="4"/>
-      <c r="B361" s="6"/>
+      <c r="B361" s="7"/>
       <c r="C361" s="4"/>
       <c r="D361" s="4"/>
       <c r="E361" s="4"/>
@@ -7865,7 +7763,7 @@
     </row>
     <row r="362" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A362" s="4"/>
-      <c r="B362" s="6"/>
+      <c r="B362" s="7"/>
       <c r="C362" s="4"/>
       <c r="D362" s="4"/>
       <c r="E362" s="4"/>
@@ -7878,7 +7776,7 @@
     </row>
     <row r="363" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A363" s="4"/>
-      <c r="B363" s="6"/>
+      <c r="B363" s="7"/>
       <c r="C363" s="4"/>
       <c r="D363" s="4"/>
       <c r="E363" s="4"/>
@@ -7891,7 +7789,7 @@
     </row>
     <row r="364" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A364" s="4"/>
-      <c r="B364" s="6"/>
+      <c r="B364" s="7"/>
       <c r="C364" s="4"/>
       <c r="D364" s="4"/>
       <c r="E364" s="4"/>
@@ -7904,7 +7802,7 @@
     </row>
     <row r="365" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A365" s="4"/>
-      <c r="B365" s="6"/>
+      <c r="B365" s="7"/>
       <c r="C365" s="4"/>
       <c r="D365" s="4"/>
       <c r="E365" s="4"/>
@@ -7917,7 +7815,7 @@
     </row>
     <row r="366" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A366" s="4"/>
-      <c r="B366" s="6"/>
+      <c r="B366" s="7"/>
       <c r="C366" s="4"/>
       <c r="D366" s="4"/>
       <c r="E366" s="4"/>
@@ -7930,7 +7828,7 @@
     </row>
     <row r="367" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A367" s="4"/>
-      <c r="B367" s="6"/>
+      <c r="B367" s="7"/>
       <c r="C367" s="4"/>
       <c r="D367" s="4"/>
       <c r="E367" s="4"/>
@@ -7943,7 +7841,7 @@
     </row>
     <row r="368" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A368" s="4"/>
-      <c r="B368" s="6"/>
+      <c r="B368" s="7"/>
       <c r="C368" s="4"/>
       <c r="D368" s="4"/>
       <c r="E368" s="4"/>
@@ -7956,7 +7854,7 @@
     </row>
     <row r="369" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A369" s="4"/>
-      <c r="B369" s="6"/>
+      <c r="B369" s="7"/>
       <c r="C369" s="4"/>
       <c r="D369" s="4"/>
       <c r="E369" s="4"/>
@@ -7969,7 +7867,7 @@
     </row>
     <row r="370" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A370" s="4"/>
-      <c r="B370" s="6"/>
+      <c r="B370" s="7"/>
       <c r="C370" s="4"/>
       <c r="D370" s="4"/>
       <c r="E370" s="4"/>
@@ -7982,7 +7880,7 @@
     </row>
     <row r="371" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A371" s="4"/>
-      <c r="B371" s="6"/>
+      <c r="B371" s="7"/>
       <c r="C371" s="4"/>
       <c r="D371" s="4"/>
       <c r="E371" s="4"/>
@@ -7995,7 +7893,7 @@
     </row>
     <row r="372" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A372" s="4"/>
-      <c r="B372" s="6"/>
+      <c r="B372" s="7"/>
       <c r="C372" s="4"/>
       <c r="D372" s="4"/>
       <c r="E372" s="4"/>
@@ -8008,7 +7906,7 @@
     </row>
     <row r="373" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A373" s="4"/>
-      <c r="B373" s="6"/>
+      <c r="B373" s="7"/>
       <c r="C373" s="4"/>
       <c r="D373" s="4"/>
       <c r="E373" s="4"/>
@@ -8021,7 +7919,7 @@
     </row>
     <row r="374" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A374" s="4"/>
-      <c r="B374" s="6"/>
+      <c r="B374" s="7"/>
       <c r="C374" s="4"/>
       <c r="D374" s="4"/>
       <c r="E374" s="4"/>
@@ -8034,7 +7932,7 @@
     </row>
     <row r="375" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A375" s="4"/>
-      <c r="B375" s="6"/>
+      <c r="B375" s="7"/>
       <c r="C375" s="4"/>
       <c r="D375" s="4"/>
       <c r="E375" s="4"/>
@@ -8047,7 +7945,7 @@
     </row>
     <row r="376" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A376" s="4"/>
-      <c r="B376" s="6"/>
+      <c r="B376" s="7"/>
       <c r="C376" s="4"/>
       <c r="D376" s="4"/>
       <c r="E376" s="4"/>
@@ -8060,7 +7958,7 @@
     </row>
     <row r="377" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A377" s="4"/>
-      <c r="B377" s="6"/>
+      <c r="B377" s="7"/>
       <c r="C377" s="4"/>
       <c r="D377" s="4"/>
       <c r="E377" s="4"/>
@@ -8073,7 +7971,7 @@
     </row>
     <row r="378" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A378" s="4"/>
-      <c r="B378" s="6"/>
+      <c r="B378" s="7"/>
       <c r="C378" s="4"/>
       <c r="D378" s="4"/>
       <c r="E378" s="4"/>
@@ -8086,7 +7984,7 @@
     </row>
     <row r="379" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A379" s="4"/>
-      <c r="B379" s="6"/>
+      <c r="B379" s="7"/>
       <c r="C379" s="4"/>
       <c r="D379" s="4"/>
       <c r="E379" s="4"/>
@@ -8099,7 +7997,7 @@
     </row>
     <row r="380" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A380" s="4"/>
-      <c r="B380" s="6"/>
+      <c r="B380" s="7"/>
       <c r="C380" s="4"/>
       <c r="D380" s="4"/>
       <c r="E380" s="4"/>
@@ -8112,7 +8010,7 @@
     </row>
     <row r="381" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A381" s="4"/>
-      <c r="B381" s="6"/>
+      <c r="B381" s="7"/>
       <c r="C381" s="4"/>
       <c r="D381" s="4"/>
       <c r="E381" s="4"/>
@@ -8125,7 +8023,7 @@
     </row>
     <row r="382" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A382" s="4"/>
-      <c r="B382" s="6"/>
+      <c r="B382" s="7"/>
       <c r="C382" s="4"/>
       <c r="D382" s="4"/>
       <c r="E382" s="4"/>
@@ -8138,7 +8036,7 @@
     </row>
     <row r="383" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A383" s="4"/>
-      <c r="B383" s="6"/>
+      <c r="B383" s="7"/>
       <c r="C383" s="4"/>
       <c r="D383" s="4"/>
       <c r="E383" s="4"/>
@@ -8151,7 +8049,7 @@
     </row>
     <row r="384" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A384" s="4"/>
-      <c r="B384" s="6"/>
+      <c r="B384" s="7"/>
       <c r="C384" s="4"/>
       <c r="D384" s="4"/>
       <c r="E384" s="4"/>
@@ -8164,7 +8062,7 @@
     </row>
     <row r="385" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A385" s="4"/>
-      <c r="B385" s="6"/>
+      <c r="B385" s="7"/>
       <c r="C385" s="4"/>
       <c r="D385" s="4"/>
       <c r="E385" s="4"/>
@@ -8177,7 +8075,7 @@
     </row>
     <row r="386" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A386" s="4"/>
-      <c r="B386" s="6"/>
+      <c r="B386" s="7"/>
       <c r="C386" s="4"/>
       <c r="D386" s="4"/>
       <c r="E386" s="4"/>
@@ -8190,7 +8088,7 @@
     </row>
     <row r="387" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A387" s="4"/>
-      <c r="B387" s="6"/>
+      <c r="B387" s="7"/>
       <c r="C387" s="4"/>
       <c r="D387" s="4"/>
       <c r="E387" s="4"/>
@@ -8203,7 +8101,7 @@
     </row>
     <row r="388" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A388" s="4"/>
-      <c r="B388" s="6"/>
+      <c r="B388" s="7"/>
       <c r="C388" s="4"/>
       <c r="D388" s="4"/>
       <c r="E388" s="4"/>
@@ -8216,7 +8114,7 @@
     </row>
     <row r="389" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A389" s="4"/>
-      <c r="B389" s="6"/>
+      <c r="B389" s="7"/>
       <c r="C389" s="4"/>
       <c r="D389" s="4"/>
       <c r="E389" s="4"/>
@@ -8229,7 +8127,7 @@
     </row>
     <row r="390" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A390" s="4"/>
-      <c r="B390" s="6"/>
+      <c r="B390" s="7"/>
       <c r="C390" s="4"/>
       <c r="D390" s="4"/>
       <c r="E390" s="4"/>
@@ -8242,7 +8140,7 @@
     </row>
     <row r="391" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A391" s="4"/>
-      <c r="B391" s="6"/>
+      <c r="B391" s="7"/>
       <c r="C391" s="4"/>
       <c r="D391" s="4"/>
       <c r="E391" s="4"/>
@@ -8255,7 +8153,7 @@
     </row>
     <row r="392" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A392" s="4"/>
-      <c r="B392" s="6"/>
+      <c r="B392" s="7"/>
       <c r="C392" s="4"/>
       <c r="D392" s="4"/>
       <c r="E392" s="4"/>
@@ -8268,7 +8166,7 @@
     </row>
     <row r="393" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A393" s="4"/>
-      <c r="B393" s="6"/>
+      <c r="B393" s="7"/>
       <c r="C393" s="4"/>
       <c r="D393" s="4"/>
       <c r="E393" s="4"/>
@@ -8281,7 +8179,7 @@
     </row>
     <row r="394" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A394" s="4"/>
-      <c r="B394" s="6"/>
+      <c r="B394" s="7"/>
       <c r="C394" s="4"/>
       <c r="D394" s="4"/>
       <c r="E394" s="4"/>
@@ -8294,7 +8192,7 @@
     </row>
     <row r="395" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A395" s="4"/>
-      <c r="B395" s="6"/>
+      <c r="B395" s="7"/>
       <c r="C395" s="4"/>
       <c r="D395" s="4"/>
       <c r="E395" s="4"/>
@@ -8307,7 +8205,7 @@
     </row>
     <row r="396" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A396" s="4"/>
-      <c r="B396" s="6"/>
+      <c r="B396" s="7"/>
       <c r="C396" s="4"/>
       <c r="D396" s="4"/>
       <c r="E396" s="4"/>
@@ -8320,7 +8218,7 @@
     </row>
     <row r="397" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A397" s="4"/>
-      <c r="B397" s="6"/>
+      <c r="B397" s="7"/>
       <c r="C397" s="4"/>
       <c r="D397" s="4"/>
       <c r="E397" s="4"/>
@@ -8333,7 +8231,7 @@
     </row>
     <row r="398" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A398" s="4"/>
-      <c r="B398" s="6"/>
+      <c r="B398" s="7"/>
       <c r="C398" s="4"/>
       <c r="D398" s="4"/>
       <c r="E398" s="4"/>
@@ -8346,7 +8244,7 @@
     </row>
     <row r="399" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A399" s="4"/>
-      <c r="B399" s="6"/>
+      <c r="B399" s="7"/>
       <c r="C399" s="4"/>
       <c r="D399" s="4"/>
       <c r="E399" s="4"/>
@@ -8359,7 +8257,7 @@
     </row>
     <row r="400" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A400" s="4"/>
-      <c r="B400" s="6"/>
+      <c r="B400" s="7"/>
       <c r="C400" s="4"/>
       <c r="D400" s="4"/>
       <c r="E400" s="4"/>
@@ -8372,7 +8270,7 @@
     </row>
     <row r="401" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A401" s="4"/>
-      <c r="B401" s="6"/>
+      <c r="B401" s="7"/>
       <c r="C401" s="4"/>
       <c r="D401" s="4"/>
       <c r="E401" s="4"/>
@@ -8385,7 +8283,7 @@
     </row>
     <row r="402" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A402" s="4"/>
-      <c r="B402" s="6"/>
+      <c r="B402" s="7"/>
       <c r="C402" s="4"/>
       <c r="D402" s="4"/>
       <c r="E402" s="4"/>

</xml_diff>